<commit_message>
19-04-2022 add download journal
</commit_message>
<xml_diff>
--- a/templates/electronicJournal.xlsx
+++ b/templates/electronicJournal.xlsx
@@ -278,50 +278,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -333,33 +293,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -578,14 +578,14 @@
   <dimension ref="A1:AN996"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21:AH21"/>
+      <selection activeCell="AA26" sqref="AA26:AH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.75" customWidth="1"/>
     <col min="2" max="22" width="2.75" customWidth="1"/>
-    <col min="23" max="24" width="2.75" style="30" customWidth="1"/>
+    <col min="23" max="24" width="2.75" style="10" customWidth="1"/>
     <col min="25" max="25" width="9.875" customWidth="1"/>
     <col min="26" max="26" width="8.625" customWidth="1"/>
     <col min="27" max="27" width="7.25" customWidth="1"/>
@@ -601,47 +601,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="24"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="6"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="7"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="22"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
@@ -649,41 +649,41 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="24"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="6"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="10"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="24"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
@@ -691,47 +691,47 @@
       <c r="AN2" s="1"/>
     </row>
     <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="15" t="s">
+      <c r="Z3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="16" t="s">
+      <c r="AA3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="17" t="s">
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="28" t="s">
         <v>6</v>
       </c>
       <c r="AJ3" s="1"/>
@@ -741,43 +741,43 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="5"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="26"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
@@ -785,42 +785,40 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
-      <c r="V5" s="36"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" s="12">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="14"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="36"/>
+      <c r="AD5" s="36"/>
+      <c r="AE5" s="36"/>
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="36"/>
+      <c r="AH5" s="37"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
@@ -830,41 +828,39 @@
     </row>
     <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="2"/>
-      <c r="AA6" s="12">
-        <v>2</v>
-      </c>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="14"/>
+      <c r="AA6" s="35"/>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="36"/>
+      <c r="AD6" s="36"/>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="36"/>
+      <c r="AG6" s="36"/>
+      <c r="AH6" s="37"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
@@ -874,41 +870,39 @@
     </row>
     <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="28"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="12">
-        <v>3</v>
-      </c>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="14"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="36"/>
+      <c r="AD7" s="36"/>
+      <c r="AE7" s="36"/>
+      <c r="AF7" s="36"/>
+      <c r="AG7" s="36"/>
+      <c r="AH7" s="37"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
@@ -918,41 +912,39 @@
     </row>
     <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="28"/>
-      <c r="X8" s="28"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="2"/>
-      <c r="AA8" s="12">
-        <v>4</v>
-      </c>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="14"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="36"/>
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="37"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
@@ -962,41 +954,39 @@
     </row>
     <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="12">
-        <v>5</v>
-      </c>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="14"/>
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="36"/>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="36"/>
+      <c r="AE9" s="36"/>
+      <c r="AF9" s="36"/>
+      <c r="AG9" s="36"/>
+      <c r="AH9" s="37"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
@@ -1006,41 +996,39 @@
     </row>
     <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
-      <c r="AA10" s="12">
-        <v>6</v>
-      </c>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="14"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="36"/>
+      <c r="AD10" s="36"/>
+      <c r="AE10" s="36"/>
+      <c r="AF10" s="36"/>
+      <c r="AG10" s="36"/>
+      <c r="AH10" s="37"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
@@ -1050,41 +1038,39 @@
     </row>
     <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="28"/>
-      <c r="X11" s="28"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="2"/>
-      <c r="AA11" s="12">
-        <v>7</v>
-      </c>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="14"/>
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="36"/>
+      <c r="AD11" s="36"/>
+      <c r="AE11" s="36"/>
+      <c r="AF11" s="36"/>
+      <c r="AG11" s="36"/>
+      <c r="AH11" s="37"/>
       <c r="AI11" s="3"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
@@ -1094,41 +1080,39 @@
     </row>
     <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="28"/>
-      <c r="X12" s="28"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="2"/>
-      <c r="AA12" s="12">
-        <v>8</v>
-      </c>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="14"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="36"/>
+      <c r="AD12" s="36"/>
+      <c r="AE12" s="36"/>
+      <c r="AF12" s="36"/>
+      <c r="AG12" s="36"/>
+      <c r="AH12" s="37"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
@@ -1138,41 +1122,39 @@
     </row>
     <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="2"/>
-      <c r="AA13" s="12">
-        <v>9</v>
-      </c>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="14"/>
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="36"/>
+      <c r="AC13" s="36"/>
+      <c r="AD13" s="36"/>
+      <c r="AE13" s="36"/>
+      <c r="AF13" s="36"/>
+      <c r="AG13" s="36"/>
+      <c r="AH13" s="37"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
@@ -1182,41 +1164,39 @@
     </row>
     <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="38"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="2"/>
-      <c r="AA14" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="13"/>
-      <c r="AH14" s="14"/>
+      <c r="AA14" s="35"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="36"/>
+      <c r="AD14" s="36"/>
+      <c r="AE14" s="36"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="36"/>
+      <c r="AH14" s="37"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
@@ -1226,41 +1206,39 @@
     </row>
     <row r="15" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="38"/>
-      <c r="U15" s="38"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="2"/>
-      <c r="AA15" s="12">
-        <v>11</v>
-      </c>
-      <c r="AB15" s="13"/>
-      <c r="AC15" s="13"/>
-      <c r="AD15" s="13"/>
-      <c r="AE15" s="13"/>
-      <c r="AF15" s="13"/>
-      <c r="AG15" s="13"/>
-      <c r="AH15" s="14"/>
+      <c r="AA15" s="35"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="36"/>
+      <c r="AD15" s="36"/>
+      <c r="AE15" s="36"/>
+      <c r="AF15" s="36"/>
+      <c r="AG15" s="36"/>
+      <c r="AH15" s="37"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
@@ -1270,41 +1248,39 @@
     </row>
     <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="38"/>
-      <c r="V16" s="38"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="2"/>
-      <c r="AA16" s="12">
-        <v>12</v>
-      </c>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13"/>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13"/>
-      <c r="AH16" s="14"/>
+      <c r="AA16" s="35"/>
+      <c r="AB16" s="36"/>
+      <c r="AC16" s="36"/>
+      <c r="AD16" s="36"/>
+      <c r="AE16" s="36"/>
+      <c r="AF16" s="36"/>
+      <c r="AG16" s="36"/>
+      <c r="AH16" s="37"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
@@ -1314,41 +1290,39 @@
     </row>
     <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="2"/>
-      <c r="AA17" s="12">
-        <v>13</v>
-      </c>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="14"/>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="36"/>
+      <c r="AC17" s="36"/>
+      <c r="AD17" s="36"/>
+      <c r="AE17" s="36"/>
+      <c r="AF17" s="36"/>
+      <c r="AG17" s="36"/>
+      <c r="AH17" s="37"/>
       <c r="AI17" s="3"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
@@ -1358,41 +1332,39 @@
     </row>
     <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
-      <c r="V18" s="38"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="2"/>
-      <c r="AA18" s="12">
-        <v>14</v>
-      </c>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13"/>
-      <c r="AH18" s="14"/>
+      <c r="AA18" s="35"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="36"/>
+      <c r="AD18" s="36"/>
+      <c r="AE18" s="36"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="36"/>
+      <c r="AH18" s="37"/>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
@@ -1402,41 +1374,39 @@
     </row>
     <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="2"/>
-      <c r="AA19" s="12">
-        <v>15</v>
-      </c>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13"/>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13"/>
-      <c r="AH19" s="14"/>
+      <c r="AA19" s="35"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AD19" s="36"/>
+      <c r="AE19" s="36"/>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="36"/>
+      <c r="AH19" s="37"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
@@ -1446,41 +1416,39 @@
     </row>
     <row r="20" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="2"/>
-      <c r="AA20" s="12">
-        <v>16</v>
-      </c>
-      <c r="AB20" s="13"/>
-      <c r="AC20" s="13"/>
-      <c r="AD20" s="13"/>
-      <c r="AE20" s="13"/>
-      <c r="AF20" s="13"/>
-      <c r="AG20" s="13"/>
-      <c r="AH20" s="14"/>
+      <c r="AA20" s="35"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="36"/>
+      <c r="AD20" s="36"/>
+      <c r="AE20" s="36"/>
+      <c r="AF20" s="36"/>
+      <c r="AG20" s="36"/>
+      <c r="AH20" s="37"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
@@ -1490,41 +1458,39 @@
     </row>
     <row r="21" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="2"/>
-      <c r="AA21" s="12">
-        <v>17</v>
-      </c>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="13"/>
-      <c r="AD21" s="13"/>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="13"/>
-      <c r="AG21" s="13"/>
-      <c r="AH21" s="14"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="36"/>
+      <c r="AD21" s="36"/>
+      <c r="AE21" s="36"/>
+      <c r="AF21" s="36"/>
+      <c r="AG21" s="36"/>
+      <c r="AH21" s="37"/>
       <c r="AI21" s="3"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
@@ -1534,41 +1500,39 @@
     </row>
     <row r="22" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="38"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="2"/>
-      <c r="AA22" s="12">
-        <v>18</v>
-      </c>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
-      <c r="AE22" s="13"/>
-      <c r="AF22" s="13"/>
-      <c r="AG22" s="13"/>
-      <c r="AH22" s="14"/>
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="36"/>
+      <c r="AD22" s="36"/>
+      <c r="AE22" s="36"/>
+      <c r="AF22" s="36"/>
+      <c r="AG22" s="36"/>
+      <c r="AH22" s="37"/>
       <c r="AI22" s="3"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
@@ -1578,41 +1542,39 @@
     </row>
     <row r="23" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="2"/>
-      <c r="AA23" s="12">
-        <v>19</v>
-      </c>
-      <c r="AB23" s="13"/>
-      <c r="AC23" s="13"/>
-      <c r="AD23" s="13"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="14"/>
+      <c r="AA23" s="35"/>
+      <c r="AB23" s="36"/>
+      <c r="AC23" s="36"/>
+      <c r="AD23" s="36"/>
+      <c r="AE23" s="36"/>
+      <c r="AF23" s="36"/>
+      <c r="AG23" s="36"/>
+      <c r="AH23" s="37"/>
       <c r="AI23" s="3"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
@@ -1622,41 +1584,39 @@
     </row>
     <row r="24" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="38"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="2"/>
-      <c r="AA24" s="12">
-        <v>20</v>
-      </c>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
-      <c r="AD24" s="13"/>
-      <c r="AE24" s="13"/>
-      <c r="AF24" s="13"/>
-      <c r="AG24" s="13"/>
-      <c r="AH24" s="14"/>
+      <c r="AA24" s="35"/>
+      <c r="AB24" s="36"/>
+      <c r="AC24" s="36"/>
+      <c r="AD24" s="36"/>
+      <c r="AE24" s="36"/>
+      <c r="AF24" s="36"/>
+      <c r="AG24" s="36"/>
+      <c r="AH24" s="37"/>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
@@ -1666,41 +1626,39 @@
     </row>
     <row r="25" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="2"/>
-      <c r="AA25" s="12">
-        <v>21</v>
-      </c>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="13"/>
-      <c r="AD25" s="13"/>
-      <c r="AE25" s="13"/>
-      <c r="AF25" s="13"/>
-      <c r="AG25" s="13"/>
-      <c r="AH25" s="14"/>
+      <c r="AA25" s="35"/>
+      <c r="AB25" s="36"/>
+      <c r="AC25" s="36"/>
+      <c r="AD25" s="36"/>
+      <c r="AE25" s="36"/>
+      <c r="AF25" s="36"/>
+      <c r="AG25" s="36"/>
+      <c r="AH25" s="37"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
@@ -1709,42 +1667,40 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="39"/>
-      <c r="T26" s="39"/>
-      <c r="U26" s="39"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="2"/>
-      <c r="AA26" s="12">
-        <v>22</v>
-      </c>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="13"/>
-      <c r="AD26" s="13"/>
-      <c r="AE26" s="13"/>
-      <c r="AF26" s="13"/>
-      <c r="AG26" s="13"/>
-      <c r="AH26" s="14"/>
+      <c r="AA26" s="35"/>
+      <c r="AB26" s="36"/>
+      <c r="AC26" s="36"/>
+      <c r="AD26" s="36"/>
+      <c r="AE26" s="36"/>
+      <c r="AF26" s="36"/>
+      <c r="AG26" s="36"/>
+      <c r="AH26" s="37"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
@@ -1753,41 +1709,39 @@
       <c r="AN26" s="1"/>
     </row>
     <row r="27" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="39"/>
-      <c r="S27" s="39"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="39"/>
-      <c r="V27" s="39"/>
-      <c r="X27" s="24"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="X27" s="6"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="2"/>
-      <c r="AA27" s="12">
-        <v>23</v>
-      </c>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="13"/>
-      <c r="AG27" s="13"/>
-      <c r="AH27" s="14"/>
+      <c r="AA27" s="35"/>
+      <c r="AB27" s="36"/>
+      <c r="AC27" s="36"/>
+      <c r="AD27" s="36"/>
+      <c r="AE27" s="36"/>
+      <c r="AF27" s="36"/>
+      <c r="AG27" s="36"/>
+      <c r="AH27" s="37"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
@@ -1796,42 +1750,40 @@
       <c r="AN27" s="1"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="39"/>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39"/>
-      <c r="V28" s="39"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="2"/>
-      <c r="AA28" s="12">
-        <v>24</v>
-      </c>
-      <c r="AB28" s="13"/>
-      <c r="AC28" s="13"/>
-      <c r="AD28" s="13"/>
-      <c r="AE28" s="13"/>
-      <c r="AF28" s="13"/>
-      <c r="AG28" s="13"/>
-      <c r="AH28" s="14"/>
+      <c r="AA28" s="35"/>
+      <c r="AB28" s="36"/>
+      <c r="AC28" s="36"/>
+      <c r="AD28" s="36"/>
+      <c r="AE28" s="36"/>
+      <c r="AF28" s="36"/>
+      <c r="AG28" s="36"/>
+      <c r="AH28" s="37"/>
       <c r="AI28" s="3"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
@@ -1840,44 +1792,42 @@
       <c r="AN28" s="1"/>
     </row>
     <row r="29" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="33"/>
-      <c r="T29" s="33"/>
-      <c r="U29" s="33"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="2"/>
-      <c r="AA29" s="12">
-        <v>25</v>
-      </c>
-      <c r="AB29" s="13"/>
-      <c r="AC29" s="13"/>
-      <c r="AD29" s="13"/>
-      <c r="AE29" s="13"/>
-      <c r="AF29" s="13"/>
-      <c r="AG29" s="13"/>
-      <c r="AH29" s="14"/>
+      <c r="AA29" s="35"/>
+      <c r="AB29" s="36"/>
+      <c r="AC29" s="36"/>
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+      <c r="AF29" s="36"/>
+      <c r="AG29" s="36"/>
+      <c r="AH29" s="37"/>
       <c r="AI29" s="3"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
@@ -1886,44 +1836,42 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="33"/>
-      <c r="V30" s="33"/>
-      <c r="W30" s="25"/>
-      <c r="X30" s="25"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+      <c r="W30" s="33"/>
+      <c r="X30" s="33"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="2"/>
-      <c r="AA30" s="12">
-        <v>26</v>
-      </c>
-      <c r="AB30" s="13"/>
-      <c r="AC30" s="13"/>
-      <c r="AD30" s="13"/>
-      <c r="AE30" s="13"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="13"/>
-      <c r="AH30" s="14"/>
+      <c r="AA30" s="35"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="37"/>
       <c r="AI30" s="3"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
@@ -1932,42 +1880,40 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="26"/>
-      <c r="X31" s="26"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="31"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="31"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="34"/>
+      <c r="X31" s="34"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="2"/>
-      <c r="AA31" s="12">
-        <v>27</v>
-      </c>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="13"/>
-      <c r="AD31" s="13"/>
-      <c r="AE31" s="13"/>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="13"/>
-      <c r="AH31" s="14"/>
+      <c r="AA31" s="35"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36"/>
+      <c r="AF31" s="36"/>
+      <c r="AG31" s="36"/>
+      <c r="AH31" s="37"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
@@ -1977,41 +1923,39 @@
     </row>
     <row r="32" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="38"/>
-      <c r="R32" s="38"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="38"/>
-      <c r="U32" s="38"/>
-      <c r="V32" s="38"/>
-      <c r="W32" s="28"/>
-      <c r="X32" s="28"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="2"/>
-      <c r="AA32" s="12">
-        <v>28</v>
-      </c>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="13"/>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="13"/>
-      <c r="AH32" s="14"/>
+      <c r="AA32" s="35"/>
+      <c r="AB32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AD32" s="36"/>
+      <c r="AE32" s="36"/>
+      <c r="AF32" s="36"/>
+      <c r="AG32" s="36"/>
+      <c r="AH32" s="37"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
@@ -2021,41 +1965,39 @@
     </row>
     <row r="33" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="38"/>
-      <c r="S33" s="38"/>
-      <c r="T33" s="38"/>
-      <c r="U33" s="38"/>
-      <c r="V33" s="38"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="2"/>
-      <c r="AA33" s="12">
-        <v>29</v>
-      </c>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13"/>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
-      <c r="AH33" s="14"/>
+      <c r="AA33" s="35"/>
+      <c r="AB33" s="36"/>
+      <c r="AC33" s="36"/>
+      <c r="AD33" s="36"/>
+      <c r="AE33" s="36"/>
+      <c r="AF33" s="36"/>
+      <c r="AG33" s="36"/>
+      <c r="AH33" s="37"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
@@ -2065,41 +2007,39 @@
     </row>
     <row r="34" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="38"/>
-      <c r="R34" s="38"/>
-      <c r="S34" s="38"/>
-      <c r="T34" s="38"/>
-      <c r="U34" s="38"/>
-      <c r="V34" s="38"/>
-      <c r="W34" s="28"/>
-      <c r="X34" s="28"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="2"/>
-      <c r="AA34" s="12">
-        <v>30</v>
-      </c>
-      <c r="AB34" s="13"/>
-      <c r="AC34" s="13"/>
-      <c r="AD34" s="13"/>
-      <c r="AE34" s="13"/>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="13"/>
-      <c r="AH34" s="14"/>
+      <c r="AA34" s="35"/>
+      <c r="AB34" s="36"/>
+      <c r="AC34" s="36"/>
+      <c r="AD34" s="36"/>
+      <c r="AE34" s="36"/>
+      <c r="AF34" s="36"/>
+      <c r="AG34" s="36"/>
+      <c r="AH34" s="37"/>
       <c r="AI34" s="3"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
@@ -2109,41 +2049,39 @@
     </row>
     <row r="35" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="38"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="38"/>
-      <c r="U35" s="38"/>
-      <c r="V35" s="38"/>
-      <c r="W35" s="28"/>
-      <c r="X35" s="28"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="2"/>
-      <c r="AA35" s="12">
-        <v>31</v>
-      </c>
-      <c r="AB35" s="13"/>
-      <c r="AC35" s="13"/>
-      <c r="AD35" s="13"/>
-      <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="13"/>
-      <c r="AH35" s="14"/>
+      <c r="AA35" s="35"/>
+      <c r="AB35" s="36"/>
+      <c r="AC35" s="36"/>
+      <c r="AD35" s="36"/>
+      <c r="AE35" s="36"/>
+      <c r="AF35" s="36"/>
+      <c r="AG35" s="36"/>
+      <c r="AH35" s="37"/>
       <c r="AI35" s="3"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
@@ -2153,41 +2091,39 @@
     </row>
     <row r="36" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
-      <c r="O36" s="38"/>
-      <c r="P36" s="38"/>
-      <c r="Q36" s="38"/>
-      <c r="R36" s="38"/>
-      <c r="S36" s="38"/>
-      <c r="T36" s="38"/>
-      <c r="U36" s="38"/>
-      <c r="V36" s="38"/>
-      <c r="W36" s="28"/>
-      <c r="X36" s="28"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="2"/>
-      <c r="AA36" s="12">
-        <v>32</v>
-      </c>
-      <c r="AB36" s="13"/>
-      <c r="AC36" s="13"/>
-      <c r="AD36" s="13"/>
-      <c r="AE36" s="13"/>
-      <c r="AF36" s="13"/>
-      <c r="AG36" s="13"/>
-      <c r="AH36" s="14"/>
+      <c r="AA36" s="35"/>
+      <c r="AB36" s="36"/>
+      <c r="AC36" s="36"/>
+      <c r="AD36" s="36"/>
+      <c r="AE36" s="36"/>
+      <c r="AF36" s="36"/>
+      <c r="AG36" s="36"/>
+      <c r="AH36" s="37"/>
       <c r="AI36" s="3"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
@@ -2197,41 +2133,39 @@
     </row>
     <row r="37" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="38"/>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="38"/>
-      <c r="U37" s="38"/>
-      <c r="V37" s="38"/>
-      <c r="W37" s="28"/>
-      <c r="X37" s="28"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="2"/>
-      <c r="AA37" s="12">
-        <v>33</v>
-      </c>
-      <c r="AB37" s="13"/>
-      <c r="AC37" s="13"/>
-      <c r="AD37" s="13"/>
-      <c r="AE37" s="13"/>
-      <c r="AF37" s="13"/>
-      <c r="AG37" s="13"/>
-      <c r="AH37" s="14"/>
+      <c r="AA37" s="35"/>
+      <c r="AB37" s="36"/>
+      <c r="AC37" s="36"/>
+      <c r="AD37" s="36"/>
+      <c r="AE37" s="36"/>
+      <c r="AF37" s="36"/>
+      <c r="AG37" s="36"/>
+      <c r="AH37" s="37"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
@@ -2241,41 +2175,39 @@
     </row>
     <row r="38" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="38"/>
-      <c r="P38" s="38"/>
-      <c r="Q38" s="38"/>
-      <c r="R38" s="38"/>
-      <c r="S38" s="38"/>
-      <c r="T38" s="38"/>
-      <c r="U38" s="38"/>
-      <c r="V38" s="38"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="2"/>
-      <c r="AA38" s="12">
-        <v>34</v>
-      </c>
-      <c r="AB38" s="13"/>
-      <c r="AC38" s="13"/>
-      <c r="AD38" s="13"/>
-      <c r="AE38" s="13"/>
-      <c r="AF38" s="13"/>
-      <c r="AG38" s="13"/>
-      <c r="AH38" s="14"/>
+      <c r="AA38" s="35"/>
+      <c r="AB38" s="36"/>
+      <c r="AC38" s="36"/>
+      <c r="AD38" s="36"/>
+      <c r="AE38" s="36"/>
+      <c r="AF38" s="36"/>
+      <c r="AG38" s="36"/>
+      <c r="AH38" s="37"/>
       <c r="AI38" s="3"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
@@ -2285,41 +2217,39 @@
     </row>
     <row r="39" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
-      <c r="N39" s="38"/>
-      <c r="O39" s="38"/>
-      <c r="P39" s="38"/>
-      <c r="Q39" s="38"/>
-      <c r="R39" s="38"/>
-      <c r="S39" s="38"/>
-      <c r="T39" s="38"/>
-      <c r="U39" s="38"/>
-      <c r="V39" s="38"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="2"/>
-      <c r="AA39" s="12">
-        <v>35</v>
-      </c>
-      <c r="AB39" s="13"/>
-      <c r="AC39" s="13"/>
-      <c r="AD39" s="13"/>
-      <c r="AE39" s="13"/>
-      <c r="AF39" s="13"/>
-      <c r="AG39" s="13"/>
-      <c r="AH39" s="14"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="36"/>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="36"/>
+      <c r="AF39" s="36"/>
+      <c r="AG39" s="36"/>
+      <c r="AH39" s="37"/>
       <c r="AI39" s="3"/>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
@@ -2329,41 +2259,39 @@
     </row>
     <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
-      <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-      <c r="P40" s="38"/>
-      <c r="Q40" s="38"/>
-      <c r="R40" s="38"/>
-      <c r="S40" s="38"/>
-      <c r="T40" s="38"/>
-      <c r="U40" s="38"/>
-      <c r="V40" s="38"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="2"/>
-      <c r="AA40" s="12">
-        <v>36</v>
-      </c>
-      <c r="AB40" s="13"/>
-      <c r="AC40" s="13"/>
-      <c r="AD40" s="13"/>
-      <c r="AE40" s="13"/>
-      <c r="AF40" s="13"/>
-      <c r="AG40" s="13"/>
-      <c r="AH40" s="14"/>
+      <c r="AA40" s="35"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="36"/>
+      <c r="AF40" s="36"/>
+      <c r="AG40" s="36"/>
+      <c r="AH40" s="37"/>
       <c r="AI40" s="3"/>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
@@ -2373,41 +2301,39 @@
     </row>
     <row r="41" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="38"/>
-      <c r="S41" s="38"/>
-      <c r="T41" s="38"/>
-      <c r="U41" s="38"/>
-      <c r="V41" s="38"/>
-      <c r="W41" s="28"/>
-      <c r="X41" s="28"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="2"/>
-      <c r="AA41" s="12">
-        <v>37</v>
-      </c>
-      <c r="AB41" s="13"/>
-      <c r="AC41" s="13"/>
-      <c r="AD41" s="13"/>
-      <c r="AE41" s="13"/>
-      <c r="AF41" s="13"/>
-      <c r="AG41" s="13"/>
-      <c r="AH41" s="14"/>
+      <c r="AA41" s="35"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AD41" s="36"/>
+      <c r="AE41" s="36"/>
+      <c r="AF41" s="36"/>
+      <c r="AG41" s="36"/>
+      <c r="AH41" s="37"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
@@ -2417,41 +2343,39 @@
     </row>
     <row r="42" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="38"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="38"/>
-      <c r="R42" s="38"/>
-      <c r="S42" s="38"/>
-      <c r="T42" s="38"/>
-      <c r="U42" s="38"/>
-      <c r="V42" s="38"/>
-      <c r="W42" s="28"/>
-      <c r="X42" s="28"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="2"/>
-      <c r="AA42" s="12">
-        <v>38</v>
-      </c>
-      <c r="AB42" s="13"/>
-      <c r="AC42" s="13"/>
-      <c r="AD42" s="13"/>
-      <c r="AE42" s="13"/>
-      <c r="AF42" s="13"/>
-      <c r="AG42" s="13"/>
-      <c r="AH42" s="14"/>
+      <c r="AA42" s="35"/>
+      <c r="AB42" s="36"/>
+      <c r="AC42" s="36"/>
+      <c r="AD42" s="36"/>
+      <c r="AE42" s="36"/>
+      <c r="AF42" s="36"/>
+      <c r="AG42" s="36"/>
+      <c r="AH42" s="37"/>
       <c r="AI42" s="3"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
@@ -2461,41 +2385,39 @@
     </row>
     <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="38"/>
-      <c r="S43" s="38"/>
-      <c r="T43" s="38"/>
-      <c r="U43" s="38"/>
-      <c r="V43" s="38"/>
-      <c r="W43" s="28"/>
-      <c r="X43" s="28"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="2"/>
-      <c r="AA43" s="12">
-        <v>39</v>
-      </c>
-      <c r="AB43" s="13"/>
-      <c r="AC43" s="13"/>
-      <c r="AD43" s="13"/>
-      <c r="AE43" s="13"/>
-      <c r="AF43" s="13"/>
-      <c r="AG43" s="13"/>
-      <c r="AH43" s="14"/>
+      <c r="AA43" s="35"/>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="36"/>
+      <c r="AD43" s="36"/>
+      <c r="AE43" s="36"/>
+      <c r="AF43" s="36"/>
+      <c r="AG43" s="36"/>
+      <c r="AH43" s="37"/>
       <c r="AI43" s="3"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
@@ -2505,41 +2427,39 @@
     </row>
     <row r="44" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="38"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
-      <c r="O44" s="38"/>
-      <c r="P44" s="38"/>
-      <c r="Q44" s="38"/>
-      <c r="R44" s="38"/>
-      <c r="S44" s="38"/>
-      <c r="T44" s="38"/>
-      <c r="U44" s="38"/>
-      <c r="V44" s="38"/>
-      <c r="W44" s="28"/>
-      <c r="X44" s="28"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="2"/>
-      <c r="AA44" s="12">
-        <v>40</v>
-      </c>
-      <c r="AB44" s="13"/>
-      <c r="AC44" s="13"/>
-      <c r="AD44" s="13"/>
-      <c r="AE44" s="13"/>
-      <c r="AF44" s="13"/>
-      <c r="AG44" s="13"/>
-      <c r="AH44" s="14"/>
+      <c r="AA44" s="35"/>
+      <c r="AB44" s="36"/>
+      <c r="AC44" s="36"/>
+      <c r="AD44" s="36"/>
+      <c r="AE44" s="36"/>
+      <c r="AF44" s="36"/>
+      <c r="AG44" s="36"/>
+      <c r="AH44" s="37"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
@@ -2549,42 +2469,40 @@
     </row>
     <row r="45" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="38"/>
-      <c r="K45" s="38"/>
-      <c r="L45" s="38"/>
-      <c r="M45" s="38"/>
-      <c r="N45" s="38"/>
-      <c r="O45" s="38"/>
-      <c r="P45" s="38"/>
-      <c r="Q45" s="38"/>
-      <c r="R45" s="38"/>
-      <c r="S45" s="38"/>
-      <c r="T45" s="38"/>
-      <c r="U45" s="38"/>
-      <c r="V45" s="38"/>
-      <c r="W45" s="28"/>
-      <c r="X45" s="28"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
       <c r="Y45" s="1"/>
-      <c r="Z45" s="40"/>
-      <c r="AA45" s="22">
-        <v>41</v>
-      </c>
-      <c r="AB45" s="6"/>
-      <c r="AC45" s="6"/>
-      <c r="AD45" s="6"/>
-      <c r="AE45" s="6"/>
-      <c r="AF45" s="6"/>
-      <c r="AG45" s="6"/>
-      <c r="AH45" s="7"/>
-      <c r="AI45" s="41"/>
+      <c r="Z45" s="14"/>
+      <c r="AA45" s="41"/>
+      <c r="AB45" s="21"/>
+      <c r="AC45" s="21"/>
+      <c r="AD45" s="21"/>
+      <c r="AE45" s="21"/>
+      <c r="AF45" s="21"/>
+      <c r="AG45" s="21"/>
+      <c r="AH45" s="22"/>
+      <c r="AI45" s="15"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
       <c r="AL45" s="1"/>
@@ -2593,42 +2511,40 @@
     </row>
     <row r="46" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="38"/>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
-      <c r="O46" s="38"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="38"/>
-      <c r="R46" s="38"/>
-      <c r="S46" s="38"/>
-      <c r="T46" s="38"/>
-      <c r="U46" s="38"/>
-      <c r="V46" s="38"/>
-      <c r="W46" s="28"/>
-      <c r="X46" s="28"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
       <c r="Y46" s="1"/>
-      <c r="Z46" s="43"/>
-      <c r="AA46" s="33">
-        <v>42</v>
-      </c>
-      <c r="AB46" s="36"/>
-      <c r="AC46" s="36"/>
-      <c r="AD46" s="36"/>
-      <c r="AE46" s="36"/>
-      <c r="AF46" s="36"/>
-      <c r="AG46" s="36"/>
-      <c r="AH46" s="36"/>
-      <c r="AI46" s="44"/>
+      <c r="Z46" s="17"/>
+      <c r="AA46" s="32"/>
+      <c r="AB46" s="31"/>
+      <c r="AC46" s="31"/>
+      <c r="AD46" s="31"/>
+      <c r="AE46" s="31"/>
+      <c r="AF46" s="31"/>
+      <c r="AG46" s="31"/>
+      <c r="AH46" s="31"/>
+      <c r="AI46" s="18"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
       <c r="AL46" s="1"/>
@@ -2637,40 +2553,40 @@
     </row>
     <row r="47" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38"/>
-      <c r="N47" s="38"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="38"/>
-      <c r="R47" s="38"/>
-      <c r="S47" s="38"/>
-      <c r="T47" s="38"/>
-      <c r="U47" s="38"/>
-      <c r="V47" s="38"/>
-      <c r="W47" s="28"/>
-      <c r="X47" s="28"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
       <c r="Y47" s="1"/>
-      <c r="Z47" s="42"/>
-      <c r="AA47" s="25"/>
-      <c r="AB47" s="26"/>
-      <c r="AC47" s="26"/>
-      <c r="AD47" s="26"/>
-      <c r="AE47" s="26"/>
-      <c r="AF47" s="26"/>
-      <c r="AG47" s="26"/>
-      <c r="AH47" s="26"/>
-      <c r="AI47" s="29"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="33"/>
+      <c r="AB47" s="34"/>
+      <c r="AC47" s="34"/>
+      <c r="AD47" s="34"/>
+      <c r="AE47" s="34"/>
+      <c r="AF47" s="34"/>
+      <c r="AG47" s="34"/>
+      <c r="AH47" s="34"/>
+      <c r="AI47" s="9"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
       <c r="AL47" s="1"/>
@@ -2679,40 +2595,40 @@
     </row>
     <row r="48" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="38"/>
-      <c r="N48" s="38"/>
-      <c r="O48" s="38"/>
-      <c r="P48" s="38"/>
-      <c r="Q48" s="38"/>
-      <c r="R48" s="38"/>
-      <c r="S48" s="38"/>
-      <c r="T48" s="38"/>
-      <c r="U48" s="38"/>
-      <c r="V48" s="38"/>
-      <c r="W48" s="28"/>
-      <c r="X48" s="28"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
       <c r="Y48" s="1"/>
-      <c r="Z48" s="20"/>
-      <c r="AA48" s="19"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="19"/>
-      <c r="AD48" s="19"/>
-      <c r="AE48" s="19"/>
-      <c r="AF48" s="19"/>
-      <c r="AG48" s="19"/>
-      <c r="AH48" s="19"/>
-      <c r="AI48" s="19"/>
+      <c r="Z48" s="42"/>
+      <c r="AA48" s="39"/>
+      <c r="AB48" s="39"/>
+      <c r="AC48" s="39"/>
+      <c r="AD48" s="39"/>
+      <c r="AE48" s="39"/>
+      <c r="AF48" s="39"/>
+      <c r="AG48" s="39"/>
+      <c r="AH48" s="39"/>
+      <c r="AI48" s="39"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
       <c r="AL48" s="1"/>
@@ -2721,50 +2637,50 @@
     </row>
     <row r="49" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="38"/>
-      <c r="N49" s="38"/>
-      <c r="O49" s="38"/>
-      <c r="P49" s="38"/>
-      <c r="Q49" s="38"/>
-      <c r="R49" s="38"/>
-      <c r="S49" s="38"/>
-      <c r="T49" s="38"/>
-      <c r="U49" s="38"/>
-      <c r="V49" s="38"/>
-      <c r="W49" s="28"/>
-      <c r="X49" s="28"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="8"/>
+      <c r="X49" s="8"/>
       <c r="Y49" s="1"/>
-      <c r="Z49" s="21" t="s">
+      <c r="Z49" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="AA49" s="7"/>
-      <c r="AB49" s="16" t="s">
+      <c r="AA49" s="22"/>
+      <c r="AB49" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AC49" s="7"/>
-      <c r="AD49" s="21" t="s">
+      <c r="AC49" s="22"/>
+      <c r="AD49" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AE49" s="7"/>
-      <c r="AF49" s="21" t="s">
+      <c r="AE49" s="22"/>
+      <c r="AF49" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AG49" s="7"/>
-      <c r="AH49" s="16" t="s">
+      <c r="AG49" s="22"/>
+      <c r="AH49" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AI49" s="7"/>
+      <c r="AI49" s="22"/>
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
       <c r="AL49" s="1"/>
@@ -2773,40 +2689,40 @@
     </row>
     <row r="50" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="38"/>
-      <c r="P50" s="38"/>
-      <c r="Q50" s="38"/>
-      <c r="R50" s="38"/>
-      <c r="S50" s="38"/>
-      <c r="T50" s="38"/>
-      <c r="U50" s="38"/>
-      <c r="V50" s="38"/>
-      <c r="W50" s="28"/>
-      <c r="X50" s="28"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="13"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
       <c r="Y50" s="1"/>
-      <c r="Z50" s="8"/>
-      <c r="AA50" s="10"/>
-      <c r="AB50" s="8"/>
-      <c r="AC50" s="10"/>
-      <c r="AD50" s="8"/>
-      <c r="AE50" s="10"/>
-      <c r="AF50" s="8"/>
-      <c r="AG50" s="10"/>
-      <c r="AH50" s="8"/>
-      <c r="AI50" s="10"/>
+      <c r="Z50" s="20"/>
+      <c r="AA50" s="24"/>
+      <c r="AB50" s="20"/>
+      <c r="AC50" s="24"/>
+      <c r="AD50" s="20"/>
+      <c r="AE50" s="24"/>
+      <c r="AF50" s="20"/>
+      <c r="AG50" s="24"/>
+      <c r="AH50" s="20"/>
+      <c r="AI50" s="24"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
       <c r="AL50" s="1"/>
@@ -2815,40 +2731,40 @@
     </row>
     <row r="51" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="38"/>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
-      <c r="M51" s="38"/>
-      <c r="N51" s="38"/>
-      <c r="O51" s="38"/>
-      <c r="P51" s="38"/>
-      <c r="Q51" s="38"/>
-      <c r="R51" s="38"/>
-      <c r="S51" s="38"/>
-      <c r="T51" s="38"/>
-      <c r="U51" s="38"/>
-      <c r="V51" s="38"/>
-      <c r="W51" s="28"/>
-      <c r="X51" s="28"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
       <c r="Y51" s="1"/>
-      <c r="Z51" s="12"/>
-      <c r="AA51" s="14"/>
-      <c r="AB51" s="12"/>
-      <c r="AC51" s="14"/>
-      <c r="AD51" s="12"/>
-      <c r="AE51" s="14"/>
-      <c r="AF51" s="12"/>
-      <c r="AG51" s="14"/>
-      <c r="AH51" s="12"/>
-      <c r="AI51" s="14"/>
+      <c r="Z51" s="35"/>
+      <c r="AA51" s="37"/>
+      <c r="AB51" s="35"/>
+      <c r="AC51" s="37"/>
+      <c r="AD51" s="35"/>
+      <c r="AE51" s="37"/>
+      <c r="AF51" s="35"/>
+      <c r="AG51" s="37"/>
+      <c r="AH51" s="35"/>
+      <c r="AI51" s="37"/>
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
       <c r="AL51" s="1"/>
@@ -2878,8 +2794,8 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
-      <c r="W52" s="29"/>
-      <c r="X52" s="29"/>
+      <c r="W52" s="9"/>
+      <c r="X52" s="9"/>
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
@@ -2920,8 +2836,8 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
-      <c r="W53" s="29"/>
-      <c r="X53" s="29"/>
+      <c r="W53" s="9"/>
+      <c r="X53" s="9"/>
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
@@ -2962,8 +2878,8 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
-      <c r="W54" s="29"/>
-      <c r="X54" s="29"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
@@ -3004,8 +2920,8 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
-      <c r="W55" s="29"/>
-      <c r="X55" s="29"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
@@ -3046,8 +2962,8 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
-      <c r="W56" s="29"/>
-      <c r="X56" s="29"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
@@ -3088,8 +3004,8 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
-      <c r="W57" s="29"/>
-      <c r="X57" s="29"/>
+      <c r="W57" s="9"/>
+      <c r="X57" s="9"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
@@ -3130,8 +3046,8 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
-      <c r="W58" s="29"/>
-      <c r="X58" s="29"/>
+      <c r="W58" s="9"/>
+      <c r="X58" s="9"/>
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
@@ -3172,8 +3088,8 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
-      <c r="W59" s="29"/>
-      <c r="X59" s="29"/>
+      <c r="W59" s="9"/>
+      <c r="X59" s="9"/>
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
@@ -3214,8 +3130,8 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
-      <c r="W60" s="29"/>
-      <c r="X60" s="29"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
@@ -3256,8 +3172,8 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
-      <c r="W61" s="29"/>
-      <c r="X61" s="29"/>
+      <c r="W61" s="9"/>
+      <c r="X61" s="9"/>
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
@@ -3298,8 +3214,8 @@
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
-      <c r="W62" s="29"/>
-      <c r="X62" s="29"/>
+      <c r="W62" s="9"/>
+      <c r="X62" s="9"/>
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
@@ -3340,8 +3256,8 @@
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
-      <c r="W63" s="29"/>
-      <c r="X63" s="29"/>
+      <c r="W63" s="9"/>
+      <c r="X63" s="9"/>
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
@@ -3382,8 +3298,8 @@
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
       <c r="V64" s="1"/>
-      <c r="W64" s="29"/>
-      <c r="X64" s="29"/>
+      <c r="W64" s="9"/>
+      <c r="X64" s="9"/>
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
@@ -3424,8 +3340,8 @@
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
-      <c r="W65" s="29"/>
-      <c r="X65" s="29"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
@@ -3466,8 +3382,8 @@
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
-      <c r="W66" s="29"/>
-      <c r="X66" s="29"/>
+      <c r="W66" s="9"/>
+      <c r="X66" s="9"/>
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
@@ -3508,8 +3424,8 @@
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
-      <c r="W67" s="29"/>
-      <c r="X67" s="29"/>
+      <c r="W67" s="9"/>
+      <c r="X67" s="9"/>
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
@@ -3550,8 +3466,8 @@
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
-      <c r="W68" s="29"/>
-      <c r="X68" s="29"/>
+      <c r="W68" s="9"/>
+      <c r="X68" s="9"/>
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
@@ -3592,8 +3508,8 @@
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
-      <c r="W69" s="29"/>
-      <c r="X69" s="29"/>
+      <c r="W69" s="9"/>
+      <c r="X69" s="9"/>
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
@@ -3634,8 +3550,8 @@
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
-      <c r="W70" s="29"/>
-      <c r="X70" s="29"/>
+      <c r="W70" s="9"/>
+      <c r="X70" s="9"/>
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
@@ -3676,8 +3592,8 @@
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
-      <c r="W71" s="29"/>
-      <c r="X71" s="29"/>
+      <c r="W71" s="9"/>
+      <c r="X71" s="9"/>
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
@@ -3718,8 +3634,8 @@
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
-      <c r="W72" s="29"/>
-      <c r="X72" s="29"/>
+      <c r="W72" s="9"/>
+      <c r="X72" s="9"/>
       <c r="Y72" s="1"/>
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
@@ -3760,8 +3676,8 @@
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
-      <c r="W73" s="29"/>
-      <c r="X73" s="29"/>
+      <c r="W73" s="9"/>
+      <c r="X73" s="9"/>
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
@@ -3802,8 +3718,8 @@
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
-      <c r="W74" s="29"/>
-      <c r="X74" s="29"/>
+      <c r="W74" s="9"/>
+      <c r="X74" s="9"/>
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
@@ -3844,8 +3760,8 @@
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
-      <c r="W75" s="29"/>
-      <c r="X75" s="29"/>
+      <c r="W75" s="9"/>
+      <c r="X75" s="9"/>
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
@@ -3886,8 +3802,8 @@
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
-      <c r="W76" s="29"/>
-      <c r="X76" s="29"/>
+      <c r="W76" s="9"/>
+      <c r="X76" s="9"/>
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
       <c r="AA76" s="1"/>
@@ -3928,8 +3844,8 @@
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
-      <c r="W77" s="29"/>
-      <c r="X77" s="29"/>
+      <c r="W77" s="9"/>
+      <c r="X77" s="9"/>
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
       <c r="AA77" s="1"/>
@@ -3970,8 +3886,8 @@
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
       <c r="V78" s="1"/>
-      <c r="W78" s="29"/>
-      <c r="X78" s="29"/>
+      <c r="W78" s="9"/>
+      <c r="X78" s="9"/>
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
       <c r="AA78" s="1"/>
@@ -4012,8 +3928,8 @@
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
       <c r="V79" s="1"/>
-      <c r="W79" s="29"/>
-      <c r="X79" s="29"/>
+      <c r="W79" s="9"/>
+      <c r="X79" s="9"/>
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
       <c r="AA79" s="1"/>
@@ -4054,8 +3970,8 @@
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
-      <c r="W80" s="29"/>
-      <c r="X80" s="29"/>
+      <c r="W80" s="9"/>
+      <c r="X80" s="9"/>
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
       <c r="AA80" s="1"/>
@@ -4096,8 +4012,8 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
-      <c r="W81" s="29"/>
-      <c r="X81" s="29"/>
+      <c r="W81" s="9"/>
+      <c r="X81" s="9"/>
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
       <c r="AA81" s="1"/>
@@ -4138,8 +4054,8 @@
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
-      <c r="W82" s="29"/>
-      <c r="X82" s="29"/>
+      <c r="W82" s="9"/>
+      <c r="X82" s="9"/>
       <c r="Y82" s="1"/>
       <c r="Z82" s="1"/>
       <c r="AA82" s="1"/>
@@ -4180,8 +4096,8 @@
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
       <c r="V83" s="1"/>
-      <c r="W83" s="29"/>
-      <c r="X83" s="29"/>
+      <c r="W83" s="9"/>
+      <c r="X83" s="9"/>
       <c r="Y83" s="1"/>
       <c r="Z83" s="1"/>
       <c r="AA83" s="1"/>
@@ -4222,8 +4138,8 @@
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
-      <c r="W84" s="29"/>
-      <c r="X84" s="29"/>
+      <c r="W84" s="9"/>
+      <c r="X84" s="9"/>
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
       <c r="AA84" s="1"/>
@@ -4264,8 +4180,8 @@
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
       <c r="V85" s="1"/>
-      <c r="W85" s="29"/>
-      <c r="X85" s="29"/>
+      <c r="W85" s="9"/>
+      <c r="X85" s="9"/>
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
       <c r="AA85" s="1"/>
@@ -4306,8 +4222,8 @@
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
-      <c r="W86" s="29"/>
-      <c r="X86" s="29"/>
+      <c r="W86" s="9"/>
+      <c r="X86" s="9"/>
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
       <c r="AA86" s="1"/>
@@ -4348,8 +4264,8 @@
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
-      <c r="W87" s="29"/>
-      <c r="X87" s="29"/>
+      <c r="W87" s="9"/>
+      <c r="X87" s="9"/>
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
       <c r="AA87" s="1"/>
@@ -4390,8 +4306,8 @@
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
-      <c r="W88" s="29"/>
-      <c r="X88" s="29"/>
+      <c r="W88" s="9"/>
+      <c r="X88" s="9"/>
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
       <c r="AA88" s="1"/>
@@ -4432,8 +4348,8 @@
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
       <c r="V89" s="1"/>
-      <c r="W89" s="29"/>
-      <c r="X89" s="29"/>
+      <c r="W89" s="9"/>
+      <c r="X89" s="9"/>
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
       <c r="AA89" s="1"/>
@@ -4474,8 +4390,8 @@
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
       <c r="V90" s="1"/>
-      <c r="W90" s="29"/>
-      <c r="X90" s="29"/>
+      <c r="W90" s="9"/>
+      <c r="X90" s="9"/>
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
       <c r="AA90" s="1"/>
@@ -4516,8 +4432,8 @@
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
       <c r="V91" s="1"/>
-      <c r="W91" s="29"/>
-      <c r="X91" s="29"/>
+      <c r="W91" s="9"/>
+      <c r="X91" s="9"/>
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
       <c r="AA91" s="1"/>
@@ -4558,8 +4474,8 @@
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
       <c r="V92" s="1"/>
-      <c r="W92" s="29"/>
-      <c r="X92" s="29"/>
+      <c r="W92" s="9"/>
+      <c r="X92" s="9"/>
       <c r="Y92" s="1"/>
       <c r="Z92" s="1"/>
       <c r="AA92" s="1"/>
@@ -4600,8 +4516,8 @@
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
       <c r="V93" s="1"/>
-      <c r="W93" s="29"/>
-      <c r="X93" s="29"/>
+      <c r="W93" s="9"/>
+      <c r="X93" s="9"/>
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
       <c r="AA93" s="1"/>
@@ -4642,8 +4558,8 @@
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
-      <c r="W94" s="29"/>
-      <c r="X94" s="29"/>
+      <c r="W94" s="9"/>
+      <c r="X94" s="9"/>
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
       <c r="AA94" s="1"/>
@@ -4684,8 +4600,8 @@
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
-      <c r="W95" s="29"/>
-      <c r="X95" s="29"/>
+      <c r="W95" s="9"/>
+      <c r="X95" s="9"/>
       <c r="Y95" s="1"/>
       <c r="Z95" s="1"/>
       <c r="AA95" s="1"/>
@@ -4726,8 +4642,8 @@
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
       <c r="V96" s="1"/>
-      <c r="W96" s="29"/>
-      <c r="X96" s="29"/>
+      <c r="W96" s="9"/>
+      <c r="X96" s="9"/>
       <c r="Y96" s="1"/>
       <c r="Z96" s="1"/>
       <c r="AA96" s="1"/>
@@ -4768,8 +4684,8 @@
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
       <c r="V97" s="1"/>
-      <c r="W97" s="29"/>
-      <c r="X97" s="29"/>
+      <c r="W97" s="9"/>
+      <c r="X97" s="9"/>
       <c r="Y97" s="1"/>
       <c r="Z97" s="1"/>
       <c r="AA97" s="1"/>
@@ -4810,8 +4726,8 @@
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
       <c r="V98" s="1"/>
-      <c r="W98" s="29"/>
-      <c r="X98" s="29"/>
+      <c r="W98" s="9"/>
+      <c r="X98" s="9"/>
       <c r="Y98" s="1"/>
       <c r="Z98" s="1"/>
       <c r="AA98" s="1"/>
@@ -4852,8 +4768,8 @@
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
       <c r="V99" s="1"/>
-      <c r="W99" s="29"/>
-      <c r="X99" s="29"/>
+      <c r="W99" s="9"/>
+      <c r="X99" s="9"/>
       <c r="Y99" s="1"/>
       <c r="Z99" s="1"/>
       <c r="AA99" s="1"/>
@@ -4894,8 +4810,8 @@
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
       <c r="V100" s="1"/>
-      <c r="W100" s="29"/>
-      <c r="X100" s="29"/>
+      <c r="W100" s="9"/>
+      <c r="X100" s="9"/>
       <c r="Y100" s="1"/>
       <c r="Z100" s="1"/>
       <c r="AA100" s="1"/>
@@ -4936,8 +4852,8 @@
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
       <c r="V101" s="1"/>
-      <c r="W101" s="29"/>
-      <c r="X101" s="29"/>
+      <c r="W101" s="9"/>
+      <c r="X101" s="9"/>
       <c r="Y101" s="1"/>
       <c r="Z101" s="1"/>
       <c r="AA101" s="1"/>
@@ -4978,8 +4894,8 @@
       <c r="T102" s="1"/>
       <c r="U102" s="1"/>
       <c r="V102" s="1"/>
-      <c r="W102" s="29"/>
-      <c r="X102" s="29"/>
+      <c r="W102" s="9"/>
+      <c r="X102" s="9"/>
       <c r="Y102" s="1"/>
       <c r="Z102" s="1"/>
       <c r="AA102" s="1"/>
@@ -5020,8 +4936,8 @@
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
-      <c r="W103" s="29"/>
-      <c r="X103" s="29"/>
+      <c r="W103" s="9"/>
+      <c r="X103" s="9"/>
       <c r="Y103" s="1"/>
       <c r="Z103" s="1"/>
       <c r="AA103" s="1"/>
@@ -5062,8 +4978,8 @@
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
       <c r="V104" s="1"/>
-      <c r="W104" s="29"/>
-      <c r="X104" s="29"/>
+      <c r="W104" s="9"/>
+      <c r="X104" s="9"/>
       <c r="Y104" s="1"/>
       <c r="Z104" s="1"/>
       <c r="AA104" s="1"/>
@@ -5104,8 +5020,8 @@
       <c r="T105" s="1"/>
       <c r="U105" s="1"/>
       <c r="V105" s="1"/>
-      <c r="W105" s="29"/>
-      <c r="X105" s="29"/>
+      <c r="W105" s="9"/>
+      <c r="X105" s="9"/>
       <c r="Y105" s="1"/>
       <c r="Z105" s="1"/>
       <c r="AA105" s="1"/>
@@ -5146,8 +5062,8 @@
       <c r="T106" s="1"/>
       <c r="U106" s="1"/>
       <c r="V106" s="1"/>
-      <c r="W106" s="29"/>
-      <c r="X106" s="29"/>
+      <c r="W106" s="9"/>
+      <c r="X106" s="9"/>
       <c r="Y106" s="1"/>
       <c r="Z106" s="1"/>
       <c r="AA106" s="1"/>
@@ -5188,8 +5104,8 @@
       <c r="T107" s="1"/>
       <c r="U107" s="1"/>
       <c r="V107" s="1"/>
-      <c r="W107" s="29"/>
-      <c r="X107" s="29"/>
+      <c r="W107" s="9"/>
+      <c r="X107" s="9"/>
       <c r="Y107" s="1"/>
       <c r="Z107" s="1"/>
       <c r="AA107" s="1"/>
@@ -5230,8 +5146,8 @@
       <c r="T108" s="1"/>
       <c r="U108" s="1"/>
       <c r="V108" s="1"/>
-      <c r="W108" s="29"/>
-      <c r="X108" s="29"/>
+      <c r="W108" s="9"/>
+      <c r="X108" s="9"/>
       <c r="Y108" s="1"/>
       <c r="Z108" s="1"/>
       <c r="AA108" s="1"/>
@@ -5272,8 +5188,8 @@
       <c r="T109" s="1"/>
       <c r="U109" s="1"/>
       <c r="V109" s="1"/>
-      <c r="W109" s="29"/>
-      <c r="X109" s="29"/>
+      <c r="W109" s="9"/>
+      <c r="X109" s="9"/>
       <c r="Y109" s="1"/>
       <c r="Z109" s="1"/>
       <c r="AA109" s="1"/>
@@ -5314,8 +5230,8 @@
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
       <c r="V110" s="1"/>
-      <c r="W110" s="29"/>
-      <c r="X110" s="29"/>
+      <c r="W110" s="9"/>
+      <c r="X110" s="9"/>
       <c r="Y110" s="1"/>
       <c r="Z110" s="1"/>
       <c r="AA110" s="1"/>
@@ -5356,8 +5272,8 @@
       <c r="T111" s="1"/>
       <c r="U111" s="1"/>
       <c r="V111" s="1"/>
-      <c r="W111" s="29"/>
-      <c r="X111" s="29"/>
+      <c r="W111" s="9"/>
+      <c r="X111" s="9"/>
       <c r="Y111" s="1"/>
       <c r="Z111" s="1"/>
       <c r="AA111" s="1"/>
@@ -5398,8 +5314,8 @@
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
       <c r="V112" s="1"/>
-      <c r="W112" s="29"/>
-      <c r="X112" s="29"/>
+      <c r="W112" s="9"/>
+      <c r="X112" s="9"/>
       <c r="Y112" s="1"/>
       <c r="Z112" s="1"/>
       <c r="AA112" s="1"/>
@@ -5440,8 +5356,8 @@
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
       <c r="V113" s="1"/>
-      <c r="W113" s="29"/>
-      <c r="X113" s="29"/>
+      <c r="W113" s="9"/>
+      <c r="X113" s="9"/>
       <c r="Y113" s="1"/>
       <c r="Z113" s="1"/>
       <c r="AA113" s="1"/>
@@ -5482,8 +5398,8 @@
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
       <c r="V114" s="1"/>
-      <c r="W114" s="29"/>
-      <c r="X114" s="29"/>
+      <c r="W114" s="9"/>
+      <c r="X114" s="9"/>
       <c r="Y114" s="1"/>
       <c r="Z114" s="1"/>
       <c r="AA114" s="1"/>
@@ -5524,8 +5440,8 @@
       <c r="T115" s="1"/>
       <c r="U115" s="1"/>
       <c r="V115" s="1"/>
-      <c r="W115" s="29"/>
-      <c r="X115" s="29"/>
+      <c r="W115" s="9"/>
+      <c r="X115" s="9"/>
       <c r="Y115" s="1"/>
       <c r="Z115" s="1"/>
       <c r="AA115" s="1"/>
@@ -5566,8 +5482,8 @@
       <c r="T116" s="1"/>
       <c r="U116" s="1"/>
       <c r="V116" s="1"/>
-      <c r="W116" s="29"/>
-      <c r="X116" s="29"/>
+      <c r="W116" s="9"/>
+      <c r="X116" s="9"/>
       <c r="Y116" s="1"/>
       <c r="Z116" s="1"/>
       <c r="AA116" s="1"/>
@@ -5608,8 +5524,8 @@
       <c r="T117" s="1"/>
       <c r="U117" s="1"/>
       <c r="V117" s="1"/>
-      <c r="W117" s="29"/>
-      <c r="X117" s="29"/>
+      <c r="W117" s="9"/>
+      <c r="X117" s="9"/>
       <c r="Y117" s="1"/>
       <c r="Z117" s="1"/>
       <c r="AA117" s="1"/>
@@ -5650,8 +5566,8 @@
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
       <c r="V118" s="1"/>
-      <c r="W118" s="29"/>
-      <c r="X118" s="29"/>
+      <c r="W118" s="9"/>
+      <c r="X118" s="9"/>
       <c r="Y118" s="1"/>
       <c r="Z118" s="1"/>
       <c r="AA118" s="1"/>
@@ -5692,8 +5608,8 @@
       <c r="T119" s="1"/>
       <c r="U119" s="1"/>
       <c r="V119" s="1"/>
-      <c r="W119" s="29"/>
-      <c r="X119" s="29"/>
+      <c r="W119" s="9"/>
+      <c r="X119" s="9"/>
       <c r="Y119" s="1"/>
       <c r="Z119" s="1"/>
       <c r="AA119" s="1"/>
@@ -5734,8 +5650,8 @@
       <c r="T120" s="1"/>
       <c r="U120" s="1"/>
       <c r="V120" s="1"/>
-      <c r="W120" s="29"/>
-      <c r="X120" s="29"/>
+      <c r="W120" s="9"/>
+      <c r="X120" s="9"/>
       <c r="Y120" s="1"/>
       <c r="Z120" s="1"/>
       <c r="AA120" s="1"/>
@@ -5776,8 +5692,8 @@
       <c r="T121" s="1"/>
       <c r="U121" s="1"/>
       <c r="V121" s="1"/>
-      <c r="W121" s="29"/>
-      <c r="X121" s="29"/>
+      <c r="W121" s="9"/>
+      <c r="X121" s="9"/>
       <c r="Y121" s="1"/>
       <c r="Z121" s="1"/>
       <c r="AA121" s="1"/>
@@ -5818,8 +5734,8 @@
       <c r="T122" s="1"/>
       <c r="U122" s="1"/>
       <c r="V122" s="1"/>
-      <c r="W122" s="29"/>
-      <c r="X122" s="29"/>
+      <c r="W122" s="9"/>
+      <c r="X122" s="9"/>
       <c r="Y122" s="1"/>
       <c r="Z122" s="1"/>
       <c r="AA122" s="1"/>
@@ -5860,8 +5776,8 @@
       <c r="T123" s="1"/>
       <c r="U123" s="1"/>
       <c r="V123" s="1"/>
-      <c r="W123" s="29"/>
-      <c r="X123" s="29"/>
+      <c r="W123" s="9"/>
+      <c r="X123" s="9"/>
       <c r="Y123" s="1"/>
       <c r="Z123" s="1"/>
       <c r="AA123" s="1"/>
@@ -5902,8 +5818,8 @@
       <c r="T124" s="1"/>
       <c r="U124" s="1"/>
       <c r="V124" s="1"/>
-      <c r="W124" s="29"/>
-      <c r="X124" s="29"/>
+      <c r="W124" s="9"/>
+      <c r="X124" s="9"/>
       <c r="Y124" s="1"/>
       <c r="Z124" s="1"/>
       <c r="AA124" s="1"/>
@@ -5944,8 +5860,8 @@
       <c r="T125" s="1"/>
       <c r="U125" s="1"/>
       <c r="V125" s="1"/>
-      <c r="W125" s="29"/>
-      <c r="X125" s="29"/>
+      <c r="W125" s="9"/>
+      <c r="X125" s="9"/>
       <c r="Y125" s="1"/>
       <c r="Z125" s="1"/>
       <c r="AA125" s="1"/>
@@ -5986,8 +5902,8 @@
       <c r="T126" s="1"/>
       <c r="U126" s="1"/>
       <c r="V126" s="1"/>
-      <c r="W126" s="29"/>
-      <c r="X126" s="29"/>
+      <c r="W126" s="9"/>
+      <c r="X126" s="9"/>
       <c r="Y126" s="1"/>
       <c r="Z126" s="1"/>
       <c r="AA126" s="1"/>
@@ -6028,8 +5944,8 @@
       <c r="T127" s="1"/>
       <c r="U127" s="1"/>
       <c r="V127" s="1"/>
-      <c r="W127" s="29"/>
-      <c r="X127" s="29"/>
+      <c r="W127" s="9"/>
+      <c r="X127" s="9"/>
       <c r="Y127" s="1"/>
       <c r="Z127" s="1"/>
       <c r="AA127" s="1"/>
@@ -6070,8 +5986,8 @@
       <c r="T128" s="1"/>
       <c r="U128" s="1"/>
       <c r="V128" s="1"/>
-      <c r="W128" s="29"/>
-      <c r="X128" s="29"/>
+      <c r="W128" s="9"/>
+      <c r="X128" s="9"/>
       <c r="Y128" s="1"/>
       <c r="Z128" s="1"/>
       <c r="AA128" s="1"/>
@@ -6112,8 +6028,8 @@
       <c r="T129" s="1"/>
       <c r="U129" s="1"/>
       <c r="V129" s="1"/>
-      <c r="W129" s="29"/>
-      <c r="X129" s="29"/>
+      <c r="W129" s="9"/>
+      <c r="X129" s="9"/>
       <c r="Y129" s="1"/>
       <c r="Z129" s="1"/>
       <c r="AA129" s="1"/>
@@ -6154,8 +6070,8 @@
       <c r="T130" s="1"/>
       <c r="U130" s="1"/>
       <c r="V130" s="1"/>
-      <c r="W130" s="29"/>
-      <c r="X130" s="29"/>
+      <c r="W130" s="9"/>
+      <c r="X130" s="9"/>
       <c r="Y130" s="1"/>
       <c r="Z130" s="1"/>
       <c r="AA130" s="1"/>
@@ -6196,8 +6112,8 @@
       <c r="T131" s="1"/>
       <c r="U131" s="1"/>
       <c r="V131" s="1"/>
-      <c r="W131" s="29"/>
-      <c r="X131" s="29"/>
+      <c r="W131" s="9"/>
+      <c r="X131" s="9"/>
       <c r="Y131" s="1"/>
       <c r="Z131" s="1"/>
       <c r="AA131" s="1"/>
@@ -6238,8 +6154,8 @@
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
       <c r="V132" s="1"/>
-      <c r="W132" s="29"/>
-      <c r="X132" s="29"/>
+      <c r="W132" s="9"/>
+      <c r="X132" s="9"/>
       <c r="Y132" s="1"/>
       <c r="Z132" s="1"/>
       <c r="AA132" s="1"/>
@@ -6280,8 +6196,8 @@
       <c r="T133" s="1"/>
       <c r="U133" s="1"/>
       <c r="V133" s="1"/>
-      <c r="W133" s="29"/>
-      <c r="X133" s="29"/>
+      <c r="W133" s="9"/>
+      <c r="X133" s="9"/>
       <c r="Y133" s="1"/>
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
@@ -6322,8 +6238,8 @@
       <c r="T134" s="1"/>
       <c r="U134" s="1"/>
       <c r="V134" s="1"/>
-      <c r="W134" s="29"/>
-      <c r="X134" s="29"/>
+      <c r="W134" s="9"/>
+      <c r="X134" s="9"/>
       <c r="Y134" s="1"/>
       <c r="Z134" s="1"/>
       <c r="AA134" s="1"/>
@@ -6364,8 +6280,8 @@
       <c r="T135" s="1"/>
       <c r="U135" s="1"/>
       <c r="V135" s="1"/>
-      <c r="W135" s="29"/>
-      <c r="X135" s="29"/>
+      <c r="W135" s="9"/>
+      <c r="X135" s="9"/>
       <c r="Y135" s="1"/>
       <c r="Z135" s="1"/>
       <c r="AA135" s="1"/>
@@ -7246,19 +7162,20 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="B3:V3"/>
-    <mergeCell ref="B26:V28"/>
     <mergeCell ref="B29:V29"/>
     <mergeCell ref="U30:U31"/>
     <mergeCell ref="AA28:AH28"/>
     <mergeCell ref="AA29:AH29"/>
     <mergeCell ref="AA30:AH30"/>
     <mergeCell ref="AA31:AH31"/>
-    <mergeCell ref="AA32:AH32"/>
-    <mergeCell ref="AA33:AH33"/>
-    <mergeCell ref="AA34:AH34"/>
-    <mergeCell ref="AA35:AH35"/>
+    <mergeCell ref="AA15:AH15"/>
+    <mergeCell ref="AA16:AH16"/>
+    <mergeCell ref="AA17:AH17"/>
+    <mergeCell ref="AA18:AH18"/>
+    <mergeCell ref="AA19:AH19"/>
+    <mergeCell ref="AA20:AH20"/>
+    <mergeCell ref="AA21:AH21"/>
+    <mergeCell ref="AA22:AH22"/>
     <mergeCell ref="J30:J31"/>
     <mergeCell ref="K30:K31"/>
     <mergeCell ref="L30:L31"/>
@@ -7298,14 +7215,6 @@
     <mergeCell ref="Z51:AA51"/>
     <mergeCell ref="AB51:AC51"/>
     <mergeCell ref="AH51:AI51"/>
-    <mergeCell ref="AA15:AH15"/>
-    <mergeCell ref="AA16:AH16"/>
-    <mergeCell ref="AA17:AH17"/>
-    <mergeCell ref="AA18:AH18"/>
-    <mergeCell ref="AA19:AH19"/>
-    <mergeCell ref="AA20:AH20"/>
-    <mergeCell ref="AA21:AH21"/>
-    <mergeCell ref="AA22:AH22"/>
     <mergeCell ref="AA42:AH42"/>
     <mergeCell ref="AA23:AH23"/>
     <mergeCell ref="AA24:AH24"/>
@@ -7318,13 +7227,10 @@
     <mergeCell ref="AA39:AH39"/>
     <mergeCell ref="AA40:AH40"/>
     <mergeCell ref="AA41:AH41"/>
-    <mergeCell ref="AA6:AH6"/>
-    <mergeCell ref="AA7:AH7"/>
-    <mergeCell ref="AA8:AH8"/>
-    <mergeCell ref="AA9:AH9"/>
-    <mergeCell ref="AA10:AH10"/>
-    <mergeCell ref="AA11:AH11"/>
-    <mergeCell ref="AA12:AH12"/>
+    <mergeCell ref="AA32:AH32"/>
+    <mergeCell ref="AA33:AH33"/>
+    <mergeCell ref="AA34:AH34"/>
+    <mergeCell ref="AA35:AH35"/>
     <mergeCell ref="AA13:AH13"/>
     <mergeCell ref="AA14:AH14"/>
     <mergeCell ref="A26:A28"/>
@@ -7336,6 +7242,14 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="B26:V28"/>
+    <mergeCell ref="AA6:AH6"/>
+    <mergeCell ref="AA7:AH7"/>
+    <mergeCell ref="AA8:AH8"/>
+    <mergeCell ref="AA9:AH9"/>
+    <mergeCell ref="AA10:AH10"/>
+    <mergeCell ref="AA11:AH11"/>
+    <mergeCell ref="AA12:AH12"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="Z1:AI2"/>
     <mergeCell ref="Z3:Z4"/>
@@ -7358,6 +7272,8 @@
     <mergeCell ref="W4:W5"/>
     <mergeCell ref="X4:X5"/>
     <mergeCell ref="AA5:AH5"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="B3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="98" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
19-04-2022 add fix download journal
</commit_message>
<xml_diff>
--- a/templates/electronicJournal.xlsx
+++ b/templates/electronicJournal.xlsx
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -304,61 +304,58 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,7 +575,7 @@
   <dimension ref="A1:AN996"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26:AH26"/>
+      <selection activeCell="B26" sqref="B26:V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,7 +598,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="43" t="s">
@@ -630,18 +627,18 @@
       <c r="W1" s="5"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="22"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="32"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
@@ -649,7 +646,7 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
       <c r="D2" s="43"/>
@@ -674,16 +671,16 @@
       <c r="W2" s="5"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="24"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="35"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
@@ -694,44 +691,44 @@
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="25" t="s">
+      <c r="Z3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="27" t="s">
+      <c r="AA3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21"/>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="28" t="s">
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="32"/>
+      <c r="AI3" s="42" t="s">
         <v>6</v>
       </c>
       <c r="AJ3" s="1"/>
@@ -741,43 +738,43 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="26"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="39"/>
+      <c r="AD4" s="39"/>
+      <c r="AE4" s="39"/>
+      <c r="AF4" s="39"/>
+      <c r="AG4" s="39"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="41"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
@@ -785,40 +782,40 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="36"/>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="36"/>
-      <c r="AE5" s="36"/>
-      <c r="AF5" s="36"/>
-      <c r="AG5" s="36"/>
-      <c r="AH5" s="37"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="23"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
@@ -853,14 +850,14 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="2"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="36"/>
-      <c r="AC6" s="36"/>
-      <c r="AD6" s="36"/>
-      <c r="AE6" s="36"/>
-      <c r="AF6" s="36"/>
-      <c r="AG6" s="36"/>
-      <c r="AH6" s="37"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="23"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
@@ -895,14 +892,14 @@
       <c r="X7" s="8"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="36"/>
-      <c r="AC7" s="36"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="36"/>
-      <c r="AF7" s="36"/>
-      <c r="AG7" s="36"/>
-      <c r="AH7" s="37"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="22"/>
+      <c r="AH7" s="23"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
@@ -937,14 +934,14 @@
       <c r="X8" s="8"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="2"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="36"/>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="36"/>
-      <c r="AF8" s="36"/>
-      <c r="AG8" s="36"/>
-      <c r="AH8" s="37"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="22"/>
+      <c r="AH8" s="23"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
@@ -979,14 +976,14 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="36"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="36"/>
-      <c r="AG9" s="36"/>
-      <c r="AH9" s="37"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="23"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
@@ -1021,14 +1018,14 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="36"/>
-      <c r="AC10" s="36"/>
-      <c r="AD10" s="36"/>
-      <c r="AE10" s="36"/>
-      <c r="AF10" s="36"/>
-      <c r="AG10" s="36"/>
-      <c r="AH10" s="37"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="23"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
@@ -1063,14 +1060,14 @@
       <c r="X11" s="8"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="2"/>
-      <c r="AA11" s="35"/>
-      <c r="AB11" s="36"/>
-      <c r="AC11" s="36"/>
-      <c r="AD11" s="36"/>
-      <c r="AE11" s="36"/>
-      <c r="AF11" s="36"/>
-      <c r="AG11" s="36"/>
-      <c r="AH11" s="37"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="22"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
+      <c r="AG11" s="22"/>
+      <c r="AH11" s="23"/>
       <c r="AI11" s="3"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
@@ -1105,14 +1102,14 @@
       <c r="X12" s="8"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="2"/>
-      <c r="AA12" s="35"/>
-      <c r="AB12" s="36"/>
-      <c r="AC12" s="36"/>
-      <c r="AD12" s="36"/>
-      <c r="AE12" s="36"/>
-      <c r="AF12" s="36"/>
-      <c r="AG12" s="36"/>
-      <c r="AH12" s="37"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="23"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
@@ -1147,14 +1144,14 @@
       <c r="X13" s="8"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="2"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="36"/>
-      <c r="AC13" s="36"/>
-      <c r="AD13" s="36"/>
-      <c r="AE13" s="36"/>
-      <c r="AF13" s="36"/>
-      <c r="AG13" s="36"/>
-      <c r="AH13" s="37"/>
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="22"/>
+      <c r="AD13" s="22"/>
+      <c r="AE13" s="22"/>
+      <c r="AF13" s="22"/>
+      <c r="AG13" s="22"/>
+      <c r="AH13" s="23"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
@@ -1189,14 +1186,14 @@
       <c r="X14" s="8"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="2"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="36"/>
-      <c r="AC14" s="36"/>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="36"/>
-      <c r="AF14" s="36"/>
-      <c r="AG14" s="36"/>
-      <c r="AH14" s="37"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="22"/>
+      <c r="AF14" s="22"/>
+      <c r="AG14" s="22"/>
+      <c r="AH14" s="23"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
@@ -1231,14 +1228,14 @@
       <c r="X15" s="8"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="2"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="36"/>
-      <c r="AC15" s="36"/>
-      <c r="AD15" s="36"/>
-      <c r="AE15" s="36"/>
-      <c r="AF15" s="36"/>
-      <c r="AG15" s="36"/>
-      <c r="AH15" s="37"/>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+      <c r="AD15" s="22"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
+      <c r="AH15" s="23"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
@@ -1273,14 +1270,14 @@
       <c r="X16" s="8"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="2"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="36"/>
-      <c r="AD16" s="36"/>
-      <c r="AE16" s="36"/>
-      <c r="AF16" s="36"/>
-      <c r="AG16" s="36"/>
-      <c r="AH16" s="37"/>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="23"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
@@ -1315,14 +1312,14 @@
       <c r="X17" s="8"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="2"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="36"/>
-      <c r="AC17" s="36"/>
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="36"/>
-      <c r="AF17" s="36"/>
-      <c r="AG17" s="36"/>
-      <c r="AH17" s="37"/>
+      <c r="AA17" s="21"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="23"/>
       <c r="AI17" s="3"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
@@ -1357,14 +1354,14 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="2"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="36"/>
-      <c r="AC18" s="36"/>
-      <c r="AD18" s="36"/>
-      <c r="AE18" s="36"/>
-      <c r="AF18" s="36"/>
-      <c r="AG18" s="36"/>
-      <c r="AH18" s="37"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="22"/>
+      <c r="AH18" s="23"/>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
@@ -1399,14 +1396,14 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="2"/>
-      <c r="AA19" s="35"/>
-      <c r="AB19" s="36"/>
-      <c r="AC19" s="36"/>
-      <c r="AD19" s="36"/>
-      <c r="AE19" s="36"/>
-      <c r="AF19" s="36"/>
-      <c r="AG19" s="36"/>
-      <c r="AH19" s="37"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
+      <c r="AG19" s="22"/>
+      <c r="AH19" s="23"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
@@ -1441,14 +1438,14 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="2"/>
-      <c r="AA20" s="35"/>
-      <c r="AB20" s="36"/>
-      <c r="AC20" s="36"/>
-      <c r="AD20" s="36"/>
-      <c r="AE20" s="36"/>
-      <c r="AF20" s="36"/>
-      <c r="AG20" s="36"/>
-      <c r="AH20" s="37"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="22"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
+      <c r="AG20" s="22"/>
+      <c r="AH20" s="23"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
@@ -1483,14 +1480,14 @@
       <c r="X21" s="8"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="2"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="36"/>
-      <c r="AE21" s="36"/>
-      <c r="AF21" s="36"/>
-      <c r="AG21" s="36"/>
-      <c r="AH21" s="37"/>
+      <c r="AA21" s="21"/>
+      <c r="AB21" s="22"/>
+      <c r="AC21" s="22"/>
+      <c r="AD21" s="22"/>
+      <c r="AE21" s="22"/>
+      <c r="AF21" s="22"/>
+      <c r="AG21" s="22"/>
+      <c r="AH21" s="23"/>
       <c r="AI21" s="3"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
@@ -1525,14 +1522,14 @@
       <c r="X22" s="8"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="2"/>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="36"/>
-      <c r="AC22" s="36"/>
-      <c r="AD22" s="36"/>
-      <c r="AE22" s="36"/>
-      <c r="AF22" s="36"/>
-      <c r="AG22" s="36"/>
-      <c r="AH22" s="37"/>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="22"/>
+      <c r="AC22" s="22"/>
+      <c r="AD22" s="22"/>
+      <c r="AE22" s="22"/>
+      <c r="AF22" s="22"/>
+      <c r="AG22" s="22"/>
+      <c r="AH22" s="23"/>
       <c r="AI22" s="3"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
@@ -1567,14 +1564,14 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="2"/>
-      <c r="AA23" s="35"/>
-      <c r="AB23" s="36"/>
-      <c r="AC23" s="36"/>
-      <c r="AD23" s="36"/>
-      <c r="AE23" s="36"/>
-      <c r="AF23" s="36"/>
-      <c r="AG23" s="36"/>
-      <c r="AH23" s="37"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="22"/>
+      <c r="AC23" s="22"/>
+      <c r="AD23" s="22"/>
+      <c r="AE23" s="22"/>
+      <c r="AF23" s="22"/>
+      <c r="AG23" s="22"/>
+      <c r="AH23" s="23"/>
       <c r="AI23" s="3"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
@@ -1609,14 +1606,14 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="2"/>
-      <c r="AA24" s="35"/>
-      <c r="AB24" s="36"/>
-      <c r="AC24" s="36"/>
-      <c r="AD24" s="36"/>
-      <c r="AE24" s="36"/>
-      <c r="AF24" s="36"/>
-      <c r="AG24" s="36"/>
-      <c r="AH24" s="37"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="22"/>
+      <c r="AD24" s="22"/>
+      <c r="AE24" s="22"/>
+      <c r="AF24" s="22"/>
+      <c r="AG24" s="22"/>
+      <c r="AH24" s="23"/>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
@@ -1651,14 +1648,14 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="2"/>
-      <c r="AA25" s="35"/>
-      <c r="AB25" s="36"/>
-      <c r="AC25" s="36"/>
-      <c r="AD25" s="36"/>
-      <c r="AE25" s="36"/>
-      <c r="AF25" s="36"/>
-      <c r="AG25" s="36"/>
-      <c r="AH25" s="37"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="22"/>
+      <c r="AD25" s="22"/>
+      <c r="AE25" s="22"/>
+      <c r="AF25" s="22"/>
+      <c r="AG25" s="22"/>
+      <c r="AH25" s="23"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
@@ -1667,40 +1664,40 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="2"/>
-      <c r="AA26" s="35"/>
-      <c r="AB26" s="36"/>
-      <c r="AC26" s="36"/>
-      <c r="AD26" s="36"/>
-      <c r="AE26" s="36"/>
-      <c r="AF26" s="36"/>
-      <c r="AG26" s="36"/>
-      <c r="AH26" s="37"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22"/>
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="22"/>
+      <c r="AH26" s="23"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
@@ -1709,39 +1706,39 @@
       <c r="AN26" s="1"/>
     </row>
     <row r="27" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="44"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="44"/>
-      <c r="T27" s="44"/>
-      <c r="U27" s="44"/>
-      <c r="V27" s="44"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
       <c r="X27" s="6"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="2"/>
-      <c r="AA27" s="35"/>
-      <c r="AB27" s="36"/>
-      <c r="AC27" s="36"/>
-      <c r="AD27" s="36"/>
-      <c r="AE27" s="36"/>
-      <c r="AF27" s="36"/>
-      <c r="AG27" s="36"/>
-      <c r="AH27" s="37"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22"/>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
+      <c r="AG27" s="22"/>
+      <c r="AH27" s="23"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
@@ -1750,40 +1747,40 @@
       <c r="AN27" s="1"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
-      <c r="P28" s="44"/>
-      <c r="Q28" s="44"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="44"/>
-      <c r="T28" s="44"/>
-      <c r="U28" s="44"/>
-      <c r="V28" s="44"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="U28" s="43"/>
+      <c r="V28" s="43"/>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="2"/>
-      <c r="AA28" s="35"/>
-      <c r="AB28" s="36"/>
-      <c r="AC28" s="36"/>
-      <c r="AD28" s="36"/>
-      <c r="AE28" s="36"/>
-      <c r="AF28" s="36"/>
-      <c r="AG28" s="36"/>
-      <c r="AH28" s="37"/>
+      <c r="AA28" s="21"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="23"/>
       <c r="AI28" s="3"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
@@ -1795,39 +1792,39 @@
       <c r="A29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="32"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
       <c r="W29" s="6"/>
       <c r="X29" s="6"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="2"/>
-      <c r="AA29" s="35"/>
-      <c r="AB29" s="36"/>
-      <c r="AC29" s="36"/>
-      <c r="AD29" s="36"/>
-      <c r="AE29" s="36"/>
-      <c r="AF29" s="36"/>
-      <c r="AG29" s="36"/>
-      <c r="AH29" s="37"/>
+      <c r="AA29" s="21"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22"/>
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="22"/>
+      <c r="AH29" s="23"/>
       <c r="AI29" s="3"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
@@ -1836,42 +1833,42 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="33"/>
-      <c r="X30" s="33"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="2"/>
-      <c r="AA30" s="35"/>
-      <c r="AB30" s="36"/>
-      <c r="AC30" s="36"/>
-      <c r="AD30" s="36"/>
-      <c r="AE30" s="36"/>
-      <c r="AF30" s="36"/>
-      <c r="AG30" s="36"/>
-      <c r="AH30" s="37"/>
+      <c r="AA30" s="21"/>
+      <c r="AB30" s="22"/>
+      <c r="AC30" s="22"/>
+      <c r="AD30" s="22"/>
+      <c r="AE30" s="22"/>
+      <c r="AF30" s="22"/>
+      <c r="AG30" s="22"/>
+      <c r="AH30" s="23"/>
       <c r="AI30" s="3"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
@@ -1880,40 +1877,40 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="31"/>
-      <c r="S31" s="31"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="31"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="34"/>
-      <c r="X31" s="34"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="27"/>
+      <c r="X31" s="27"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="2"/>
-      <c r="AA31" s="35"/>
-      <c r="AB31" s="36"/>
-      <c r="AC31" s="36"/>
-      <c r="AD31" s="36"/>
-      <c r="AE31" s="36"/>
-      <c r="AF31" s="36"/>
-      <c r="AG31" s="36"/>
-      <c r="AH31" s="37"/>
+      <c r="AA31" s="21"/>
+      <c r="AB31" s="22"/>
+      <c r="AC31" s="22"/>
+      <c r="AD31" s="22"/>
+      <c r="AE31" s="22"/>
+      <c r="AF31" s="22"/>
+      <c r="AG31" s="22"/>
+      <c r="AH31" s="23"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
@@ -1948,14 +1945,14 @@
       <c r="X32" s="8"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="2"/>
-      <c r="AA32" s="35"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="36"/>
-      <c r="AD32" s="36"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="36"/>
-      <c r="AG32" s="36"/>
-      <c r="AH32" s="37"/>
+      <c r="AA32" s="21"/>
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="22"/>
+      <c r="AD32" s="22"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="22"/>
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="23"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
@@ -1990,14 +1987,14 @@
       <c r="X33" s="8"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="2"/>
-      <c r="AA33" s="35"/>
-      <c r="AB33" s="36"/>
-      <c r="AC33" s="36"/>
-      <c r="AD33" s="36"/>
-      <c r="AE33" s="36"/>
-      <c r="AF33" s="36"/>
-      <c r="AG33" s="36"/>
-      <c r="AH33" s="37"/>
+      <c r="AA33" s="21"/>
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="22"/>
+      <c r="AG33" s="22"/>
+      <c r="AH33" s="23"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
@@ -2032,14 +2029,14 @@
       <c r="X34" s="8"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="2"/>
-      <c r="AA34" s="35"/>
-      <c r="AB34" s="36"/>
-      <c r="AC34" s="36"/>
-      <c r="AD34" s="36"/>
-      <c r="AE34" s="36"/>
-      <c r="AF34" s="36"/>
-      <c r="AG34" s="36"/>
-      <c r="AH34" s="37"/>
+      <c r="AA34" s="21"/>
+      <c r="AB34" s="22"/>
+      <c r="AC34" s="22"/>
+      <c r="AD34" s="22"/>
+      <c r="AE34" s="22"/>
+      <c r="AF34" s="22"/>
+      <c r="AG34" s="22"/>
+      <c r="AH34" s="23"/>
       <c r="AI34" s="3"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
@@ -2074,14 +2071,14 @@
       <c r="X35" s="8"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="2"/>
-      <c r="AA35" s="35"/>
-      <c r="AB35" s="36"/>
-      <c r="AC35" s="36"/>
-      <c r="AD35" s="36"/>
-      <c r="AE35" s="36"/>
-      <c r="AF35" s="36"/>
-      <c r="AG35" s="36"/>
-      <c r="AH35" s="37"/>
+      <c r="AA35" s="21"/>
+      <c r="AB35" s="22"/>
+      <c r="AC35" s="22"/>
+      <c r="AD35" s="22"/>
+      <c r="AE35" s="22"/>
+      <c r="AF35" s="22"/>
+      <c r="AG35" s="22"/>
+      <c r="AH35" s="23"/>
       <c r="AI35" s="3"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
@@ -2116,14 +2113,14 @@
       <c r="X36" s="8"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="2"/>
-      <c r="AA36" s="35"/>
-      <c r="AB36" s="36"/>
-      <c r="AC36" s="36"/>
-      <c r="AD36" s="36"/>
-      <c r="AE36" s="36"/>
-      <c r="AF36" s="36"/>
-      <c r="AG36" s="36"/>
-      <c r="AH36" s="37"/>
+      <c r="AA36" s="21"/>
+      <c r="AB36" s="22"/>
+      <c r="AC36" s="22"/>
+      <c r="AD36" s="22"/>
+      <c r="AE36" s="22"/>
+      <c r="AF36" s="22"/>
+      <c r="AG36" s="22"/>
+      <c r="AH36" s="23"/>
       <c r="AI36" s="3"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
@@ -2158,14 +2155,14 @@
       <c r="X37" s="8"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="2"/>
-      <c r="AA37" s="35"/>
-      <c r="AB37" s="36"/>
-      <c r="AC37" s="36"/>
-      <c r="AD37" s="36"/>
-      <c r="AE37" s="36"/>
-      <c r="AF37" s="36"/>
-      <c r="AG37" s="36"/>
-      <c r="AH37" s="37"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="22"/>
+      <c r="AC37" s="22"/>
+      <c r="AD37" s="22"/>
+      <c r="AE37" s="22"/>
+      <c r="AF37" s="22"/>
+      <c r="AG37" s="22"/>
+      <c r="AH37" s="23"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
@@ -2200,14 +2197,14 @@
       <c r="X38" s="8"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="2"/>
-      <c r="AA38" s="35"/>
-      <c r="AB38" s="36"/>
-      <c r="AC38" s="36"/>
-      <c r="AD38" s="36"/>
-      <c r="AE38" s="36"/>
-      <c r="AF38" s="36"/>
-      <c r="AG38" s="36"/>
-      <c r="AH38" s="37"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="22"/>
+      <c r="AC38" s="22"/>
+      <c r="AD38" s="22"/>
+      <c r="AE38" s="22"/>
+      <c r="AF38" s="22"/>
+      <c r="AG38" s="22"/>
+      <c r="AH38" s="23"/>
       <c r="AI38" s="3"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
@@ -2242,14 +2239,14 @@
       <c r="X39" s="8"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="2"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="36"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="36"/>
-      <c r="AE39" s="36"/>
-      <c r="AF39" s="36"/>
-      <c r="AG39" s="36"/>
-      <c r="AH39" s="37"/>
+      <c r="AA39" s="21"/>
+      <c r="AB39" s="22"/>
+      <c r="AC39" s="22"/>
+      <c r="AD39" s="22"/>
+      <c r="AE39" s="22"/>
+      <c r="AF39" s="22"/>
+      <c r="AG39" s="22"/>
+      <c r="AH39" s="23"/>
       <c r="AI39" s="3"/>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
@@ -2284,14 +2281,14 @@
       <c r="X40" s="8"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="2"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="36"/>
-      <c r="AE40" s="36"/>
-      <c r="AF40" s="36"/>
-      <c r="AG40" s="36"/>
-      <c r="AH40" s="37"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="22"/>
+      <c r="AC40" s="22"/>
+      <c r="AD40" s="22"/>
+      <c r="AE40" s="22"/>
+      <c r="AF40" s="22"/>
+      <c r="AG40" s="22"/>
+      <c r="AH40" s="23"/>
       <c r="AI40" s="3"/>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
@@ -2326,14 +2323,14 @@
       <c r="X41" s="8"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="2"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="36"/>
-      <c r="AC41" s="36"/>
-      <c r="AD41" s="36"/>
-      <c r="AE41" s="36"/>
-      <c r="AF41" s="36"/>
-      <c r="AG41" s="36"/>
-      <c r="AH41" s="37"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="22"/>
+      <c r="AC41" s="22"/>
+      <c r="AD41" s="22"/>
+      <c r="AE41" s="22"/>
+      <c r="AF41" s="22"/>
+      <c r="AG41" s="22"/>
+      <c r="AH41" s="23"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
@@ -2368,14 +2365,14 @@
       <c r="X42" s="8"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="2"/>
-      <c r="AA42" s="35"/>
-      <c r="AB42" s="36"/>
-      <c r="AC42" s="36"/>
-      <c r="AD42" s="36"/>
-      <c r="AE42" s="36"/>
-      <c r="AF42" s="36"/>
-      <c r="AG42" s="36"/>
-      <c r="AH42" s="37"/>
+      <c r="AA42" s="21"/>
+      <c r="AB42" s="22"/>
+      <c r="AC42" s="22"/>
+      <c r="AD42" s="22"/>
+      <c r="AE42" s="22"/>
+      <c r="AF42" s="22"/>
+      <c r="AG42" s="22"/>
+      <c r="AH42" s="23"/>
       <c r="AI42" s="3"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
@@ -2410,14 +2407,14 @@
       <c r="X43" s="8"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="2"/>
-      <c r="AA43" s="35"/>
-      <c r="AB43" s="36"/>
-      <c r="AC43" s="36"/>
-      <c r="AD43" s="36"/>
-      <c r="AE43" s="36"/>
-      <c r="AF43" s="36"/>
-      <c r="AG43" s="36"/>
-      <c r="AH43" s="37"/>
+      <c r="AA43" s="21"/>
+      <c r="AB43" s="22"/>
+      <c r="AC43" s="22"/>
+      <c r="AD43" s="22"/>
+      <c r="AE43" s="22"/>
+      <c r="AF43" s="22"/>
+      <c r="AG43" s="22"/>
+      <c r="AH43" s="23"/>
       <c r="AI43" s="3"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
@@ -2452,14 +2449,14 @@
       <c r="X44" s="8"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="2"/>
-      <c r="AA44" s="35"/>
-      <c r="AB44" s="36"/>
-      <c r="AC44" s="36"/>
-      <c r="AD44" s="36"/>
-      <c r="AE44" s="36"/>
-      <c r="AF44" s="36"/>
-      <c r="AG44" s="36"/>
-      <c r="AH44" s="37"/>
+      <c r="AA44" s="21"/>
+      <c r="AB44" s="22"/>
+      <c r="AC44" s="22"/>
+      <c r="AD44" s="22"/>
+      <c r="AE44" s="22"/>
+      <c r="AF44" s="22"/>
+      <c r="AG44" s="22"/>
+      <c r="AH44" s="23"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
@@ -2494,14 +2491,14 @@
       <c r="X45" s="8"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="14"/>
-      <c r="AA45" s="41"/>
-      <c r="AB45" s="21"/>
-      <c r="AC45" s="21"/>
-      <c r="AD45" s="21"/>
-      <c r="AE45" s="21"/>
-      <c r="AF45" s="21"/>
-      <c r="AG45" s="21"/>
-      <c r="AH45" s="22"/>
+      <c r="AA45" s="30"/>
+      <c r="AB45" s="31"/>
+      <c r="AC45" s="31"/>
+      <c r="AD45" s="31"/>
+      <c r="AE45" s="31"/>
+      <c r="AF45" s="31"/>
+      <c r="AG45" s="31"/>
+      <c r="AH45" s="32"/>
       <c r="AI45" s="15"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
@@ -2536,14 +2533,14 @@
       <c r="X46" s="8"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="17"/>
-      <c r="AA46" s="32"/>
-      <c r="AB46" s="31"/>
-      <c r="AC46" s="31"/>
-      <c r="AD46" s="31"/>
-      <c r="AE46" s="31"/>
-      <c r="AF46" s="31"/>
-      <c r="AG46" s="31"/>
-      <c r="AH46" s="31"/>
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="20"/>
+      <c r="AC46" s="20"/>
+      <c r="AD46" s="20"/>
+      <c r="AE46" s="20"/>
+      <c r="AF46" s="20"/>
+      <c r="AG46" s="20"/>
+      <c r="AH46" s="20"/>
       <c r="AI46" s="18"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
@@ -2578,14 +2575,14 @@
       <c r="X47" s="8"/>
       <c r="Y47" s="1"/>
       <c r="Z47" s="16"/>
-      <c r="AA47" s="33"/>
-      <c r="AB47" s="34"/>
-      <c r="AC47" s="34"/>
-      <c r="AD47" s="34"/>
-      <c r="AE47" s="34"/>
-      <c r="AF47" s="34"/>
-      <c r="AG47" s="34"/>
-      <c r="AH47" s="34"/>
+      <c r="AA47" s="26"/>
+      <c r="AB47" s="27"/>
+      <c r="AC47" s="27"/>
+      <c r="AD47" s="27"/>
+      <c r="AE47" s="27"/>
+      <c r="AF47" s="27"/>
+      <c r="AG47" s="27"/>
+      <c r="AH47" s="27"/>
       <c r="AI47" s="9"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
@@ -2619,16 +2616,16 @@
       <c r="W48" s="8"/>
       <c r="X48" s="8"/>
       <c r="Y48" s="1"/>
-      <c r="Z48" s="42"/>
-      <c r="AA48" s="39"/>
-      <c r="AB48" s="39"/>
-      <c r="AC48" s="39"/>
-      <c r="AD48" s="39"/>
-      <c r="AE48" s="39"/>
-      <c r="AF48" s="39"/>
-      <c r="AG48" s="39"/>
-      <c r="AH48" s="39"/>
-      <c r="AI48" s="39"/>
+      <c r="Z48" s="33"/>
+      <c r="AA48" s="34"/>
+      <c r="AB48" s="34"/>
+      <c r="AC48" s="34"/>
+      <c r="AD48" s="34"/>
+      <c r="AE48" s="34"/>
+      <c r="AF48" s="34"/>
+      <c r="AG48" s="34"/>
+      <c r="AH48" s="34"/>
+      <c r="AI48" s="34"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
       <c r="AL48" s="1"/>
@@ -2661,26 +2658,26 @@
       <c r="W49" s="8"/>
       <c r="X49" s="8"/>
       <c r="Y49" s="1"/>
-      <c r="Z49" s="29" t="s">
+      <c r="Z49" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AA49" s="22"/>
-      <c r="AB49" s="27" t="s">
+      <c r="AA49" s="32"/>
+      <c r="AB49" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="AC49" s="22"/>
-      <c r="AD49" s="29" t="s">
+      <c r="AC49" s="32"/>
+      <c r="AD49" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="AE49" s="22"/>
-      <c r="AF49" s="29" t="s">
+      <c r="AE49" s="32"/>
+      <c r="AF49" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="AG49" s="22"/>
-      <c r="AH49" s="27" t="s">
+      <c r="AG49" s="32"/>
+      <c r="AH49" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AI49" s="22"/>
+      <c r="AI49" s="32"/>
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
       <c r="AL49" s="1"/>
@@ -2713,16 +2710,16 @@
       <c r="W50" s="8"/>
       <c r="X50" s="8"/>
       <c r="Y50" s="1"/>
-      <c r="Z50" s="20"/>
-      <c r="AA50" s="24"/>
-      <c r="AB50" s="20"/>
-      <c r="AC50" s="24"/>
-      <c r="AD50" s="20"/>
-      <c r="AE50" s="24"/>
-      <c r="AF50" s="20"/>
-      <c r="AG50" s="24"/>
-      <c r="AH50" s="20"/>
-      <c r="AI50" s="24"/>
+      <c r="Z50" s="29"/>
+      <c r="AA50" s="35"/>
+      <c r="AB50" s="29"/>
+      <c r="AC50" s="35"/>
+      <c r="AD50" s="29"/>
+      <c r="AE50" s="35"/>
+      <c r="AF50" s="29"/>
+      <c r="AG50" s="35"/>
+      <c r="AH50" s="29"/>
+      <c r="AI50" s="35"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
       <c r="AL50" s="1"/>
@@ -2755,16 +2752,16 @@
       <c r="W51" s="8"/>
       <c r="X51" s="8"/>
       <c r="Y51" s="1"/>
-      <c r="Z51" s="35"/>
-      <c r="AA51" s="37"/>
-      <c r="AB51" s="35"/>
-      <c r="AC51" s="37"/>
-      <c r="AD51" s="35"/>
-      <c r="AE51" s="37"/>
-      <c r="AF51" s="35"/>
-      <c r="AG51" s="37"/>
-      <c r="AH51" s="35"/>
-      <c r="AI51" s="37"/>
+      <c r="Z51" s="21"/>
+      <c r="AA51" s="23"/>
+      <c r="AB51" s="21"/>
+      <c r="AC51" s="23"/>
+      <c r="AD51" s="21"/>
+      <c r="AE51" s="23"/>
+      <c r="AF51" s="21"/>
+      <c r="AG51" s="23"/>
+      <c r="AH51" s="21"/>
+      <c r="AI51" s="23"/>
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
       <c r="AL51" s="1"/>
@@ -7162,6 +7159,94 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="112">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Z1:AI2"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="AA5:AH5"/>
+    <mergeCell ref="B1:V2"/>
+    <mergeCell ref="B3:V3"/>
+    <mergeCell ref="AA13:AH13"/>
+    <mergeCell ref="AA14:AH14"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="B26:V28"/>
+    <mergeCell ref="AA6:AH6"/>
+    <mergeCell ref="AA7:AH7"/>
+    <mergeCell ref="AA8:AH8"/>
+    <mergeCell ref="AA9:AH9"/>
+    <mergeCell ref="AA10:AH10"/>
+    <mergeCell ref="AA11:AH11"/>
+    <mergeCell ref="AA12:AH12"/>
+    <mergeCell ref="AA42:AH42"/>
+    <mergeCell ref="AA23:AH23"/>
+    <mergeCell ref="AA24:AH24"/>
+    <mergeCell ref="AA25:AH25"/>
+    <mergeCell ref="AA26:AH26"/>
+    <mergeCell ref="AA27:AH27"/>
+    <mergeCell ref="AA36:AH36"/>
+    <mergeCell ref="AA37:AH37"/>
+    <mergeCell ref="AA38:AH38"/>
+    <mergeCell ref="AA39:AH39"/>
+    <mergeCell ref="AA40:AH40"/>
+    <mergeCell ref="AA41:AH41"/>
+    <mergeCell ref="AA32:AH32"/>
+    <mergeCell ref="AA33:AH33"/>
+    <mergeCell ref="AA34:AH34"/>
+    <mergeCell ref="AA35:AH35"/>
+    <mergeCell ref="AA43:AH43"/>
+    <mergeCell ref="AA44:AH44"/>
+    <mergeCell ref="AA45:AH45"/>
+    <mergeCell ref="AA46:AH46"/>
+    <mergeCell ref="AA47:AH47"/>
+    <mergeCell ref="Z48:AI48"/>
+    <mergeCell ref="AD51:AE51"/>
+    <mergeCell ref="AF51:AG51"/>
+    <mergeCell ref="Z49:AA50"/>
+    <mergeCell ref="AB49:AC50"/>
+    <mergeCell ref="AD49:AE50"/>
+    <mergeCell ref="AF49:AG50"/>
+    <mergeCell ref="AH49:AI50"/>
+    <mergeCell ref="Z51:AA51"/>
+    <mergeCell ref="AB51:AC51"/>
+    <mergeCell ref="AH51:AI51"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="R30:R31"/>
+    <mergeCell ref="S30:S31"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
     <mergeCell ref="B29:V29"/>
     <mergeCell ref="U30:U31"/>
     <mergeCell ref="AA28:AH28"/>
@@ -7186,94 +7271,6 @@
     <mergeCell ref="X30:X31"/>
     <mergeCell ref="O30:O31"/>
     <mergeCell ref="P30:P31"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="R30:R31"/>
-    <mergeCell ref="S30:S31"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="AA43:AH43"/>
-    <mergeCell ref="AA44:AH44"/>
-    <mergeCell ref="AA45:AH45"/>
-    <mergeCell ref="AA46:AH46"/>
-    <mergeCell ref="AA47:AH47"/>
-    <mergeCell ref="Z48:AI48"/>
-    <mergeCell ref="AD51:AE51"/>
-    <mergeCell ref="AF51:AG51"/>
-    <mergeCell ref="Z49:AA50"/>
-    <mergeCell ref="AB49:AC50"/>
-    <mergeCell ref="AD49:AE50"/>
-    <mergeCell ref="AF49:AG50"/>
-    <mergeCell ref="AH49:AI50"/>
-    <mergeCell ref="Z51:AA51"/>
-    <mergeCell ref="AB51:AC51"/>
-    <mergeCell ref="AH51:AI51"/>
-    <mergeCell ref="AA42:AH42"/>
-    <mergeCell ref="AA23:AH23"/>
-    <mergeCell ref="AA24:AH24"/>
-    <mergeCell ref="AA25:AH25"/>
-    <mergeCell ref="AA26:AH26"/>
-    <mergeCell ref="AA27:AH27"/>
-    <mergeCell ref="AA36:AH36"/>
-    <mergeCell ref="AA37:AH37"/>
-    <mergeCell ref="AA38:AH38"/>
-    <mergeCell ref="AA39:AH39"/>
-    <mergeCell ref="AA40:AH40"/>
-    <mergeCell ref="AA41:AH41"/>
-    <mergeCell ref="AA32:AH32"/>
-    <mergeCell ref="AA33:AH33"/>
-    <mergeCell ref="AA34:AH34"/>
-    <mergeCell ref="AA35:AH35"/>
-    <mergeCell ref="AA13:AH13"/>
-    <mergeCell ref="AA14:AH14"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="B26:V28"/>
-    <mergeCell ref="AA6:AH6"/>
-    <mergeCell ref="AA7:AH7"/>
-    <mergeCell ref="AA8:AH8"/>
-    <mergeCell ref="AA9:AH9"/>
-    <mergeCell ref="AA10:AH10"/>
-    <mergeCell ref="AA11:AH11"/>
-    <mergeCell ref="AA12:AH12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Z1:AI2"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="AA5:AH5"/>
-    <mergeCell ref="B1:V2"/>
-    <mergeCell ref="B3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="98" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
21-04-2022 add fix download electronic journal
</commit_message>
<xml_diff>
--- a/templates/electronicJournal.xlsx
+++ b/templates/electronicJournal.xlsx
@@ -46,19 +46,19 @@
     <t>дата (дд) Фамилия,Имя_обучающегося</t>
   </si>
   <si>
-    <t>№ Приказа о зачислении</t>
-  </si>
-  <si>
     <t>Дата защиты</t>
-  </si>
-  <si>
-    <t>№ приказа об отчислении</t>
   </si>
   <si>
     <t>Объем услуги  (чел*час)</t>
   </si>
   <si>
     <t>Подпись</t>
+  </si>
+  <si>
+    <t>№ Приказа о формировании группы</t>
+  </si>
+  <si>
+    <t>№ приказа о завершении группы</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +91,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
@@ -270,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -308,11 +321,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,14 +336,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -343,9 +354,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -354,7 +366,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -574,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN996"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:V28"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="AD49" sqref="AD49:AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -598,46 +649,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
       <c r="W1" s="5"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="38" t="s">
+      <c r="Z1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
       <c r="AI1" s="32"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
@@ -646,41 +697,41 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
       <c r="W2" s="5"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="35"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="33"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
@@ -715,20 +766,20 @@
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="40" t="s">
+      <c r="Z3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="36" t="s">
+      <c r="AA3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="31"/>
-      <c r="AG3" s="31"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
       <c r="AH3" s="32"/>
-      <c r="AI3" s="42" t="s">
+      <c r="AI3" s="41" t="s">
         <v>6</v>
       </c>
       <c r="AJ3" s="1"/>
@@ -738,43 +789,43 @@
       <c r="AN3" s="1"/>
     </row>
     <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
       <c r="U4" s="19"/>
       <c r="V4" s="19"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="39"/>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="35"/>
-      <c r="AI4" s="41"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="40"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
@@ -782,7 +833,7 @@
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -804,18 +855,18 @@
       <c r="T5" s="20"/>
       <c r="U5" s="20"/>
       <c r="V5" s="20"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="23"/>
+      <c r="AA5" s="50"/>
+      <c r="AB5" s="51"/>
+      <c r="AC5" s="51"/>
+      <c r="AD5" s="51"/>
+      <c r="AE5" s="51"/>
+      <c r="AF5" s="51"/>
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="52"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
@@ -850,14 +901,14 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="2"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="23"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="51"/>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="51"/>
+      <c r="AE6" s="51"/>
+      <c r="AF6" s="51"/>
+      <c r="AG6" s="51"/>
+      <c r="AH6" s="52"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
@@ -892,14 +943,14 @@
       <c r="X7" s="8"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="23"/>
+      <c r="AA7" s="50"/>
+      <c r="AB7" s="51"/>
+      <c r="AC7" s="51"/>
+      <c r="AD7" s="51"/>
+      <c r="AE7" s="51"/>
+      <c r="AF7" s="51"/>
+      <c r="AG7" s="51"/>
+      <c r="AH7" s="52"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
@@ -934,14 +985,14 @@
       <c r="X8" s="8"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="2"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
-      <c r="AG8" s="22"/>
-      <c r="AH8" s="23"/>
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="51"/>
+      <c r="AC8" s="51"/>
+      <c r="AD8" s="51"/>
+      <c r="AE8" s="51"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="52"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
@@ -976,14 +1027,14 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="23"/>
+      <c r="AA9" s="50"/>
+      <c r="AB9" s="51"/>
+      <c r="AC9" s="51"/>
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="51"/>
+      <c r="AF9" s="51"/>
+      <c r="AG9" s="51"/>
+      <c r="AH9" s="52"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
@@ -1018,14 +1069,14 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="22"/>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="22"/>
-      <c r="AG10" s="22"/>
-      <c r="AH10" s="23"/>
+      <c r="AA10" s="50"/>
+      <c r="AB10" s="51"/>
+      <c r="AC10" s="51"/>
+      <c r="AD10" s="51"/>
+      <c r="AE10" s="51"/>
+      <c r="AF10" s="51"/>
+      <c r="AG10" s="51"/>
+      <c r="AH10" s="52"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
@@ -1060,14 +1111,14 @@
       <c r="X11" s="8"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="2"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-      <c r="AG11" s="22"/>
-      <c r="AH11" s="23"/>
+      <c r="AA11" s="50"/>
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="51"/>
+      <c r="AD11" s="51"/>
+      <c r="AE11" s="51"/>
+      <c r="AF11" s="51"/>
+      <c r="AG11" s="51"/>
+      <c r="AH11" s="52"/>
       <c r="AI11" s="3"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
@@ -1102,14 +1153,14 @@
       <c r="X12" s="8"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="2"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="22"/>
-      <c r="AD12" s="22"/>
-      <c r="AE12" s="22"/>
-      <c r="AF12" s="22"/>
-      <c r="AG12" s="22"/>
-      <c r="AH12" s="23"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="51"/>
+      <c r="AD12" s="51"/>
+      <c r="AE12" s="51"/>
+      <c r="AF12" s="51"/>
+      <c r="AG12" s="51"/>
+      <c r="AH12" s="52"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
@@ -1144,14 +1195,14 @@
       <c r="X13" s="8"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="2"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="22"/>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="22"/>
-      <c r="AE13" s="22"/>
-      <c r="AF13" s="22"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="23"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="51"/>
+      <c r="AC13" s="51"/>
+      <c r="AD13" s="51"/>
+      <c r="AE13" s="51"/>
+      <c r="AF13" s="51"/>
+      <c r="AG13" s="51"/>
+      <c r="AH13" s="52"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
@@ -1186,14 +1237,14 @@
       <c r="X14" s="8"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="2"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="22"/>
-      <c r="AC14" s="22"/>
-      <c r="AD14" s="22"/>
-      <c r="AE14" s="22"/>
-      <c r="AF14" s="22"/>
-      <c r="AG14" s="22"/>
-      <c r="AH14" s="23"/>
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="52"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
@@ -1228,14 +1279,14 @@
       <c r="X15" s="8"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="2"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="22"/>
-      <c r="AC15" s="22"/>
-      <c r="AD15" s="22"/>
-      <c r="AE15" s="22"/>
-      <c r="AF15" s="22"/>
-      <c r="AG15" s="22"/>
-      <c r="AH15" s="23"/>
+      <c r="AA15" s="50"/>
+      <c r="AB15" s="51"/>
+      <c r="AC15" s="51"/>
+      <c r="AD15" s="51"/>
+      <c r="AE15" s="51"/>
+      <c r="AF15" s="51"/>
+      <c r="AG15" s="51"/>
+      <c r="AH15" s="52"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
@@ -1270,14 +1321,14 @@
       <c r="X16" s="8"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="2"/>
-      <c r="AA16" s="21"/>
-      <c r="AB16" s="22"/>
-      <c r="AC16" s="22"/>
-      <c r="AD16" s="22"/>
-      <c r="AE16" s="22"/>
-      <c r="AF16" s="22"/>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="23"/>
+      <c r="AA16" s="50"/>
+      <c r="AB16" s="51"/>
+      <c r="AC16" s="51"/>
+      <c r="AD16" s="51"/>
+      <c r="AE16" s="51"/>
+      <c r="AF16" s="51"/>
+      <c r="AG16" s="51"/>
+      <c r="AH16" s="52"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
@@ -1312,14 +1363,14 @@
       <c r="X17" s="8"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="2"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="22"/>
-      <c r="AC17" s="22"/>
-      <c r="AD17" s="22"/>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
-      <c r="AG17" s="22"/>
-      <c r="AH17" s="23"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="51"/>
+      <c r="AG17" s="51"/>
+      <c r="AH17" s="52"/>
       <c r="AI17" s="3"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
@@ -1354,14 +1405,14 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="2"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22"/>
-      <c r="AE18" s="22"/>
-      <c r="AF18" s="22"/>
-      <c r="AG18" s="22"/>
-      <c r="AH18" s="23"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="51"/>
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="51"/>
+      <c r="AF18" s="51"/>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="52"/>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
@@ -1396,14 +1447,14 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="2"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="22"/>
-      <c r="AC19" s="22"/>
-      <c r="AD19" s="22"/>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
-      <c r="AG19" s="22"/>
-      <c r="AH19" s="23"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="52"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
@@ -1438,14 +1489,14 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="2"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22"/>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
-      <c r="AG20" s="22"/>
-      <c r="AH20" s="23"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="52"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
@@ -1480,14 +1531,14 @@
       <c r="X21" s="8"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="2"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="22"/>
-      <c r="AC21" s="22"/>
-      <c r="AD21" s="22"/>
-      <c r="AE21" s="22"/>
-      <c r="AF21" s="22"/>
-      <c r="AG21" s="22"/>
-      <c r="AH21" s="23"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="51"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="51"/>
+      <c r="AF21" s="51"/>
+      <c r="AG21" s="51"/>
+      <c r="AH21" s="52"/>
       <c r="AI21" s="3"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
@@ -1522,14 +1573,14 @@
       <c r="X22" s="8"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="2"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="22"/>
-      <c r="AC22" s="22"/>
-      <c r="AD22" s="22"/>
-      <c r="AE22" s="22"/>
-      <c r="AF22" s="22"/>
-      <c r="AG22" s="22"/>
-      <c r="AH22" s="23"/>
+      <c r="AA22" s="50"/>
+      <c r="AB22" s="51"/>
+      <c r="AC22" s="51"/>
+      <c r="AD22" s="51"/>
+      <c r="AE22" s="51"/>
+      <c r="AF22" s="51"/>
+      <c r="AG22" s="51"/>
+      <c r="AH22" s="52"/>
       <c r="AI22" s="3"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
@@ -1564,14 +1615,14 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="2"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="22"/>
-      <c r="AC23" s="22"/>
-      <c r="AD23" s="22"/>
-      <c r="AE23" s="22"/>
-      <c r="AF23" s="22"/>
-      <c r="AG23" s="22"/>
-      <c r="AH23" s="23"/>
+      <c r="AA23" s="50"/>
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="52"/>
       <c r="AI23" s="3"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
@@ -1606,14 +1657,14 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="2"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="22"/>
-      <c r="AC24" s="22"/>
-      <c r="AD24" s="22"/>
-      <c r="AE24" s="22"/>
-      <c r="AF24" s="22"/>
-      <c r="AG24" s="22"/>
-      <c r="AH24" s="23"/>
+      <c r="AA24" s="50"/>
+      <c r="AB24" s="51"/>
+      <c r="AC24" s="51"/>
+      <c r="AD24" s="51"/>
+      <c r="AE24" s="51"/>
+      <c r="AF24" s="51"/>
+      <c r="AG24" s="51"/>
+      <c r="AH24" s="52"/>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
@@ -1648,14 +1699,14 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="2"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="22"/>
-      <c r="AC25" s="22"/>
-      <c r="AD25" s="22"/>
-      <c r="AE25" s="22"/>
-      <c r="AF25" s="22"/>
-      <c r="AG25" s="22"/>
-      <c r="AH25" s="23"/>
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="51"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+      <c r="AE25" s="51"/>
+      <c r="AF25" s="51"/>
+      <c r="AG25" s="51"/>
+      <c r="AH25" s="52"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
@@ -1664,40 +1715,40 @@
       <c r="AN25" s="1"/>
     </row>
     <row r="26" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="43"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="36"/>
+      <c r="V26" s="36"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="2"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="22"/>
-      <c r="AC26" s="22"/>
-      <c r="AD26" s="22"/>
-      <c r="AE26" s="22"/>
-      <c r="AF26" s="22"/>
-      <c r="AG26" s="22"/>
-      <c r="AH26" s="23"/>
+      <c r="AA26" s="50"/>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="52"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
@@ -1706,39 +1757,39 @@
       <c r="AN26" s="1"/>
     </row>
     <row r="27" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="34"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="36"/>
+      <c r="V27" s="36"/>
       <c r="X27" s="6"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="2"/>
-      <c r="AA27" s="21"/>
-      <c r="AB27" s="22"/>
-      <c r="AC27" s="22"/>
-      <c r="AD27" s="22"/>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
-      <c r="AG27" s="22"/>
-      <c r="AH27" s="23"/>
+      <c r="AA27" s="50"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="51"/>
+      <c r="AG27" s="51"/>
+      <c r="AH27" s="52"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
@@ -1747,40 +1798,40 @@
       <c r="AN27" s="1"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="43"/>
-      <c r="R28" s="43"/>
-      <c r="S28" s="43"/>
-      <c r="T28" s="43"/>
-      <c r="U28" s="43"/>
-      <c r="V28" s="43"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="36"/>
+      <c r="V28" s="36"/>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="2"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="23"/>
+      <c r="AA28" s="50"/>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="51"/>
+      <c r="AF28" s="51"/>
+      <c r="AG28" s="51"/>
+      <c r="AH28" s="52"/>
       <c r="AI28" s="3"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
@@ -1817,14 +1868,14 @@
       <c r="X29" s="6"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="2"/>
-      <c r="AA29" s="21"/>
-      <c r="AB29" s="22"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22"/>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22"/>
-      <c r="AH29" s="23"/>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AF29" s="51"/>
+      <c r="AG29" s="51"/>
+      <c r="AH29" s="52"/>
       <c r="AI29" s="3"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
@@ -1833,42 +1884,42 @@
       <c r="AN29" s="1"/>
     </row>
     <row r="30" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
       <c r="U30" s="19"/>
       <c r="V30" s="19"/>
-      <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="2"/>
-      <c r="AA30" s="21"/>
-      <c r="AB30" s="22"/>
-      <c r="AC30" s="22"/>
-      <c r="AD30" s="22"/>
-      <c r="AE30" s="22"/>
-      <c r="AF30" s="22"/>
-      <c r="AG30" s="22"/>
-      <c r="AH30" s="23"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="52"/>
       <c r="AI30" s="3"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
@@ -1877,7 +1928,7 @@
       <c r="AN30" s="1"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -1899,18 +1950,18 @@
       <c r="T31" s="20"/>
       <c r="U31" s="20"/>
       <c r="V31" s="20"/>
-      <c r="W31" s="27"/>
-      <c r="X31" s="27"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="2"/>
-      <c r="AA31" s="21"/>
-      <c r="AB31" s="22"/>
-      <c r="AC31" s="22"/>
-      <c r="AD31" s="22"/>
-      <c r="AE31" s="22"/>
-      <c r="AF31" s="22"/>
-      <c r="AG31" s="22"/>
-      <c r="AH31" s="23"/>
+      <c r="AA31" s="50"/>
+      <c r="AB31" s="51"/>
+      <c r="AC31" s="51"/>
+      <c r="AD31" s="51"/>
+      <c r="AE31" s="51"/>
+      <c r="AF31" s="51"/>
+      <c r="AG31" s="51"/>
+      <c r="AH31" s="52"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
@@ -1945,14 +1996,14 @@
       <c r="X32" s="8"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="2"/>
-      <c r="AA32" s="21"/>
-      <c r="AB32" s="22"/>
-      <c r="AC32" s="22"/>
-      <c r="AD32" s="22"/>
-      <c r="AE32" s="22"/>
-      <c r="AF32" s="22"/>
-      <c r="AG32" s="22"/>
-      <c r="AH32" s="23"/>
+      <c r="AA32" s="50"/>
+      <c r="AB32" s="51"/>
+      <c r="AC32" s="51"/>
+      <c r="AD32" s="51"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="51"/>
+      <c r="AG32" s="51"/>
+      <c r="AH32" s="52"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
@@ -1987,14 +2038,14 @@
       <c r="X33" s="8"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="2"/>
-      <c r="AA33" s="21"/>
-      <c r="AB33" s="22"/>
-      <c r="AC33" s="22"/>
-      <c r="AD33" s="22"/>
-      <c r="AE33" s="22"/>
-      <c r="AF33" s="22"/>
-      <c r="AG33" s="22"/>
-      <c r="AH33" s="23"/>
+      <c r="AA33" s="50"/>
+      <c r="AB33" s="51"/>
+      <c r="AC33" s="51"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="51"/>
+      <c r="AF33" s="51"/>
+      <c r="AG33" s="51"/>
+      <c r="AH33" s="52"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
@@ -2029,14 +2080,14 @@
       <c r="X34" s="8"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="2"/>
-      <c r="AA34" s="21"/>
-      <c r="AB34" s="22"/>
-      <c r="AC34" s="22"/>
-      <c r="AD34" s="22"/>
-      <c r="AE34" s="22"/>
-      <c r="AF34" s="22"/>
-      <c r="AG34" s="22"/>
-      <c r="AH34" s="23"/>
+      <c r="AA34" s="50"/>
+      <c r="AB34" s="51"/>
+      <c r="AC34" s="51"/>
+      <c r="AD34" s="51"/>
+      <c r="AE34" s="51"/>
+      <c r="AF34" s="51"/>
+      <c r="AG34" s="51"/>
+      <c r="AH34" s="52"/>
       <c r="AI34" s="3"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
@@ -2071,14 +2122,14 @@
       <c r="X35" s="8"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="2"/>
-      <c r="AA35" s="21"/>
-      <c r="AB35" s="22"/>
-      <c r="AC35" s="22"/>
-      <c r="AD35" s="22"/>
-      <c r="AE35" s="22"/>
-      <c r="AF35" s="22"/>
-      <c r="AG35" s="22"/>
-      <c r="AH35" s="23"/>
+      <c r="AA35" s="50"/>
+      <c r="AB35" s="51"/>
+      <c r="AC35" s="51"/>
+      <c r="AD35" s="51"/>
+      <c r="AE35" s="51"/>
+      <c r="AF35" s="51"/>
+      <c r="AG35" s="51"/>
+      <c r="AH35" s="52"/>
       <c r="AI35" s="3"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
@@ -2113,14 +2164,14 @@
       <c r="X36" s="8"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="2"/>
-      <c r="AA36" s="21"/>
-      <c r="AB36" s="22"/>
-      <c r="AC36" s="22"/>
-      <c r="AD36" s="22"/>
-      <c r="AE36" s="22"/>
-      <c r="AF36" s="22"/>
-      <c r="AG36" s="22"/>
-      <c r="AH36" s="23"/>
+      <c r="AA36" s="50"/>
+      <c r="AB36" s="51"/>
+      <c r="AC36" s="51"/>
+      <c r="AD36" s="51"/>
+      <c r="AE36" s="51"/>
+      <c r="AF36" s="51"/>
+      <c r="AG36" s="51"/>
+      <c r="AH36" s="52"/>
       <c r="AI36" s="3"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
@@ -2155,14 +2206,14 @@
       <c r="X37" s="8"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="2"/>
-      <c r="AA37" s="21"/>
-      <c r="AB37" s="22"/>
-      <c r="AC37" s="22"/>
-      <c r="AD37" s="22"/>
-      <c r="AE37" s="22"/>
-      <c r="AF37" s="22"/>
-      <c r="AG37" s="22"/>
-      <c r="AH37" s="23"/>
+      <c r="AA37" s="50"/>
+      <c r="AB37" s="51"/>
+      <c r="AC37" s="51"/>
+      <c r="AD37" s="51"/>
+      <c r="AE37" s="51"/>
+      <c r="AF37" s="51"/>
+      <c r="AG37" s="51"/>
+      <c r="AH37" s="52"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
@@ -2197,14 +2248,14 @@
       <c r="X38" s="8"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="2"/>
-      <c r="AA38" s="21"/>
-      <c r="AB38" s="22"/>
-      <c r="AC38" s="22"/>
-      <c r="AD38" s="22"/>
-      <c r="AE38" s="22"/>
-      <c r="AF38" s="22"/>
-      <c r="AG38" s="22"/>
-      <c r="AH38" s="23"/>
+      <c r="AA38" s="50"/>
+      <c r="AB38" s="51"/>
+      <c r="AC38" s="51"/>
+      <c r="AD38" s="51"/>
+      <c r="AE38" s="51"/>
+      <c r="AF38" s="51"/>
+      <c r="AG38" s="51"/>
+      <c r="AH38" s="52"/>
       <c r="AI38" s="3"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
@@ -2239,14 +2290,14 @@
       <c r="X39" s="8"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="2"/>
-      <c r="AA39" s="21"/>
-      <c r="AB39" s="22"/>
-      <c r="AC39" s="22"/>
-      <c r="AD39" s="22"/>
-      <c r="AE39" s="22"/>
-      <c r="AF39" s="22"/>
-      <c r="AG39" s="22"/>
-      <c r="AH39" s="23"/>
+      <c r="AA39" s="50"/>
+      <c r="AB39" s="51"/>
+      <c r="AC39" s="51"/>
+      <c r="AD39" s="51"/>
+      <c r="AE39" s="51"/>
+      <c r="AF39" s="51"/>
+      <c r="AG39" s="51"/>
+      <c r="AH39" s="52"/>
       <c r="AI39" s="3"/>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
@@ -2281,14 +2332,14 @@
       <c r="X40" s="8"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="2"/>
-      <c r="AA40" s="21"/>
-      <c r="AB40" s="22"/>
-      <c r="AC40" s="22"/>
-      <c r="AD40" s="22"/>
-      <c r="AE40" s="22"/>
-      <c r="AF40" s="22"/>
-      <c r="AG40" s="22"/>
-      <c r="AH40" s="23"/>
+      <c r="AA40" s="50"/>
+      <c r="AB40" s="51"/>
+      <c r="AC40" s="51"/>
+      <c r="AD40" s="51"/>
+      <c r="AE40" s="51"/>
+      <c r="AF40" s="51"/>
+      <c r="AG40" s="51"/>
+      <c r="AH40" s="52"/>
       <c r="AI40" s="3"/>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
@@ -2323,14 +2374,14 @@
       <c r="X41" s="8"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="2"/>
-      <c r="AA41" s="21"/>
-      <c r="AB41" s="22"/>
-      <c r="AC41" s="22"/>
-      <c r="AD41" s="22"/>
-      <c r="AE41" s="22"/>
-      <c r="AF41" s="22"/>
-      <c r="AG41" s="22"/>
-      <c r="AH41" s="23"/>
+      <c r="AA41" s="50"/>
+      <c r="AB41" s="51"/>
+      <c r="AC41" s="51"/>
+      <c r="AD41" s="51"/>
+      <c r="AE41" s="51"/>
+      <c r="AF41" s="51"/>
+      <c r="AG41" s="51"/>
+      <c r="AH41" s="52"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
@@ -2365,14 +2416,14 @@
       <c r="X42" s="8"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="2"/>
-      <c r="AA42" s="21"/>
-      <c r="AB42" s="22"/>
-      <c r="AC42" s="22"/>
-      <c r="AD42" s="22"/>
-      <c r="AE42" s="22"/>
-      <c r="AF42" s="22"/>
-      <c r="AG42" s="22"/>
-      <c r="AH42" s="23"/>
+      <c r="AA42" s="50"/>
+      <c r="AB42" s="51"/>
+      <c r="AC42" s="51"/>
+      <c r="AD42" s="51"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="51"/>
+      <c r="AG42" s="51"/>
+      <c r="AH42" s="52"/>
       <c r="AI42" s="3"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
@@ -2407,14 +2458,14 @@
       <c r="X43" s="8"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="2"/>
-      <c r="AA43" s="21"/>
-      <c r="AB43" s="22"/>
-      <c r="AC43" s="22"/>
-      <c r="AD43" s="22"/>
-      <c r="AE43" s="22"/>
-      <c r="AF43" s="22"/>
-      <c r="AG43" s="22"/>
-      <c r="AH43" s="23"/>
+      <c r="AA43" s="50"/>
+      <c r="AB43" s="51"/>
+      <c r="AC43" s="51"/>
+      <c r="AD43" s="51"/>
+      <c r="AE43" s="51"/>
+      <c r="AF43" s="51"/>
+      <c r="AG43" s="51"/>
+      <c r="AH43" s="52"/>
       <c r="AI43" s="3"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
@@ -2449,14 +2500,14 @@
       <c r="X44" s="8"/>
       <c r="Y44" s="1"/>
       <c r="Z44" s="2"/>
-      <c r="AA44" s="21"/>
-      <c r="AB44" s="22"/>
-      <c r="AC44" s="22"/>
-      <c r="AD44" s="22"/>
-      <c r="AE44" s="22"/>
-      <c r="AF44" s="22"/>
-      <c r="AG44" s="22"/>
-      <c r="AH44" s="23"/>
+      <c r="AA44" s="50"/>
+      <c r="AB44" s="51"/>
+      <c r="AC44" s="51"/>
+      <c r="AD44" s="51"/>
+      <c r="AE44" s="51"/>
+      <c r="AF44" s="51"/>
+      <c r="AG44" s="51"/>
+      <c r="AH44" s="52"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
@@ -2491,14 +2542,14 @@
       <c r="X45" s="8"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="14"/>
-      <c r="AA45" s="30"/>
-      <c r="AB45" s="31"/>
-      <c r="AC45" s="31"/>
-      <c r="AD45" s="31"/>
-      <c r="AE45" s="31"/>
-      <c r="AF45" s="31"/>
-      <c r="AG45" s="31"/>
-      <c r="AH45" s="32"/>
+      <c r="AA45" s="53"/>
+      <c r="AB45" s="54"/>
+      <c r="AC45" s="54"/>
+      <c r="AD45" s="54"/>
+      <c r="AE45" s="54"/>
+      <c r="AF45" s="54"/>
+      <c r="AG45" s="54"/>
+      <c r="AH45" s="55"/>
       <c r="AI45" s="15"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
@@ -2533,14 +2584,14 @@
       <c r="X46" s="8"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="17"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="20"/>
-      <c r="AC46" s="20"/>
-      <c r="AD46" s="20"/>
-      <c r="AE46" s="20"/>
-      <c r="AF46" s="20"/>
-      <c r="AG46" s="20"/>
-      <c r="AH46" s="20"/>
+      <c r="AA46" s="56"/>
+      <c r="AB46" s="57"/>
+      <c r="AC46" s="57"/>
+      <c r="AD46" s="57"/>
+      <c r="AE46" s="57"/>
+      <c r="AF46" s="57"/>
+      <c r="AG46" s="57"/>
+      <c r="AH46" s="57"/>
       <c r="AI46" s="18"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
@@ -2575,14 +2626,14 @@
       <c r="X47" s="8"/>
       <c r="Y47" s="1"/>
       <c r="Z47" s="16"/>
-      <c r="AA47" s="26"/>
-      <c r="AB47" s="27"/>
-      <c r="AC47" s="27"/>
-      <c r="AD47" s="27"/>
-      <c r="AE47" s="27"/>
-      <c r="AF47" s="27"/>
-      <c r="AG47" s="27"/>
-      <c r="AH47" s="27"/>
+      <c r="AA47" s="23"/>
+      <c r="AB47" s="24"/>
+      <c r="AC47" s="24"/>
+      <c r="AD47" s="24"/>
+      <c r="AE47" s="24"/>
+      <c r="AF47" s="24"/>
+      <c r="AG47" s="24"/>
+      <c r="AH47" s="24"/>
       <c r="AI47" s="9"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
@@ -2616,16 +2667,16 @@
       <c r="W48" s="8"/>
       <c r="X48" s="8"/>
       <c r="Y48" s="1"/>
-      <c r="Z48" s="33"/>
-      <c r="AA48" s="34"/>
-      <c r="AB48" s="34"/>
-      <c r="AC48" s="34"/>
-      <c r="AD48" s="34"/>
-      <c r="AE48" s="34"/>
-      <c r="AF48" s="34"/>
-      <c r="AG48" s="34"/>
-      <c r="AH48" s="34"/>
-      <c r="AI48" s="34"/>
+      <c r="Z48" s="28"/>
+      <c r="AA48" s="29"/>
+      <c r="AB48" s="29"/>
+      <c r="AC48" s="29"/>
+      <c r="AD48" s="29"/>
+      <c r="AE48" s="29"/>
+      <c r="AF48" s="29"/>
+      <c r="AG48" s="29"/>
+      <c r="AH48" s="29"/>
+      <c r="AI48" s="29"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
       <c r="AL48" s="1"/>
@@ -2658,24 +2709,24 @@
       <c r="W49" s="8"/>
       <c r="X49" s="8"/>
       <c r="Y49" s="1"/>
-      <c r="Z49" s="28" t="s">
+      <c r="Z49" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA49" s="46"/>
+      <c r="AB49" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="AA49" s="32"/>
-      <c r="AB49" s="36" t="s">
+      <c r="AC49" s="42"/>
+      <c r="AD49" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE49" s="46"/>
+      <c r="AF49" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="AC49" s="32"/>
-      <c r="AD49" s="28" t="s">
+      <c r="AG49" s="46"/>
+      <c r="AH49" s="34" t="s">
         <v>10</v>
-      </c>
-      <c r="AE49" s="32"/>
-      <c r="AF49" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG49" s="32"/>
-      <c r="AH49" s="36" t="s">
-        <v>12</v>
       </c>
       <c r="AI49" s="32"/>
       <c r="AJ49" s="1"/>
@@ -2710,16 +2761,16 @@
       <c r="W50" s="8"/>
       <c r="X50" s="8"/>
       <c r="Y50" s="1"/>
-      <c r="Z50" s="29"/>
-      <c r="AA50" s="35"/>
-      <c r="AB50" s="29"/>
-      <c r="AC50" s="35"/>
-      <c r="AD50" s="29"/>
-      <c r="AE50" s="35"/>
-      <c r="AF50" s="29"/>
-      <c r="AG50" s="35"/>
-      <c r="AH50" s="29"/>
-      <c r="AI50" s="35"/>
+      <c r="Z50" s="47"/>
+      <c r="AA50" s="48"/>
+      <c r="AB50" s="43"/>
+      <c r="AC50" s="44"/>
+      <c r="AD50" s="47"/>
+      <c r="AE50" s="48"/>
+      <c r="AF50" s="47"/>
+      <c r="AG50" s="48"/>
+      <c r="AH50" s="26"/>
+      <c r="AI50" s="33"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
       <c r="AL50" s="1"/>
@@ -2752,16 +2803,16 @@
       <c r="W51" s="8"/>
       <c r="X51" s="8"/>
       <c r="Y51" s="1"/>
-      <c r="Z51" s="21"/>
-      <c r="AA51" s="23"/>
-      <c r="AB51" s="21"/>
-      <c r="AC51" s="23"/>
-      <c r="AD51" s="21"/>
-      <c r="AE51" s="23"/>
-      <c r="AF51" s="21"/>
-      <c r="AG51" s="23"/>
-      <c r="AH51" s="21"/>
-      <c r="AI51" s="23"/>
+      <c r="Z51" s="30"/>
+      <c r="AA51" s="31"/>
+      <c r="AB51" s="30"/>
+      <c r="AC51" s="31"/>
+      <c r="AD51" s="30"/>
+      <c r="AE51" s="31"/>
+      <c r="AF51" s="30"/>
+      <c r="AG51" s="31"/>
+      <c r="AH51" s="30"/>
+      <c r="AI51" s="31"/>
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
       <c r="AL51" s="1"/>

</xml_diff>